<commit_message>
Initial commit on develop branch
</commit_message>
<xml_diff>
--- a/6.Gerenciamento de Projeto/SYLF - Planejamento e Controle do Projeto.xlsx
+++ b/6.Gerenciamento de Projeto/SYLF - Planejamento e Controle do Projeto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\School\6 semestre\ESO\SYLF\6.Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1A3F59D-F579-41E7-B810-A7448EF400D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E1C61E-F125-45D0-AB70-1D3DA1CA4BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="4" xr2:uid="{31237A52-FFD1-4E1D-B5BB-391D11929C61}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{31237A52-FFD1-4E1D-B5BB-391D11929C61}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -4741,7 +4741,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="231">
   <si>
     <t>Equipe</t>
   </si>
@@ -5502,9 +5502,6 @@
     <t>Especificar, Analisar e Projetar  UC1 -  Realizar inicialização e parada emergencial de modo sem fio.</t>
   </si>
   <si>
-    <t>Especificar, Analisar e Projetar UC2 - Monitorar o estado dos componentes que compoem o robô.</t>
-  </si>
-  <si>
     <t>Modelar,implementar e testar a arquitetura de UC1</t>
   </si>
   <si>
@@ -5514,49 +5511,19 @@
     <t>Implementar e testar a arquitetura de UC1</t>
   </si>
   <si>
-    <t>Modelar,implementar e testar a arquitetura de UC2</t>
-  </si>
-  <si>
-    <t>Criar Guia de Implementação de UC2</t>
-  </si>
-  <si>
-    <t>Implementar e testar a arquitetura de UC2</t>
-  </si>
-  <si>
-    <t>Especificar, Analisar e Projetar  UC3 - Alterar valores de variáveis de código de modo sem fio.</t>
-  </si>
-  <si>
-    <t>Modelar,implementar e testar a arquitetura de UC3</t>
-  </si>
-  <si>
-    <t>Criar Guia de Implementação de UC3</t>
-  </si>
-  <si>
-    <t>Implementar e testar a arquitetura de UC3</t>
-  </si>
-  <si>
-    <t>Modelar o UC1 -  Realizar inicialização e parada emergencial de modo sem fio.</t>
-  </si>
-  <si>
-    <t>Modelar, Implementart e Testar o UC1 -  Realizar inicialização e parada emergencial de modo sem fio.</t>
-  </si>
-  <si>
-    <t>Modelar o UC2 - Monitorar o estado dos componentes que compoem o robô.</t>
-  </si>
-  <si>
-    <t>Modelar, Implementart e Testar o UC2 - Monitorar o estado dos componentes que compoem o robô.</t>
-  </si>
-  <si>
-    <t>Modelar o UC3 - Alterar valores de variáveis de código de modo sem fio.</t>
-  </si>
-  <si>
-    <t>Modelar, Implementart e Testar o UC3 - Alterar valores de variáveis de código de modo sem fio.</t>
-  </si>
-  <si>
     <t>21/8/2025</t>
   </si>
   <si>
     <t>Release- 1.1.1</t>
+  </si>
+  <si>
+    <t>Desenvolver o UC1 -  Realizar inicialização e parada emergencial de modo sem fio.</t>
+  </si>
+  <si>
+    <t>Desenvolver o UC2 - Monitorar o estado dos componentes que compoem o robô.</t>
+  </si>
+  <si>
+    <t>Desenvolver o UC3 - Alterar valores de variáveis de código de modo sem fio.</t>
   </si>
 </sst>
 </file>
@@ -6137,7 +6104,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6197,10 +6164,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="9" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -6513,6 +6476,52 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="168" fontId="21" fillId="6" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="17" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="17" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="9" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="40" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6524,6 +6533,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="10" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="9" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6546,6 +6567,18 @@
     <xf numFmtId="164" fontId="22" fillId="5" borderId="7" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="171" fontId="40" fillId="9" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="9" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="9" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="27" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6572,6 +6605,9 @@
     <xf numFmtId="164" fontId="32" fillId="15" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="31" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="32" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6584,9 +6620,6 @@
     <xf numFmtId="164" fontId="31" fillId="14" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6616,76 +6649,6 @@
     </xf>
     <xf numFmtId="164" fontId="30" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="10" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="9" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="17" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="17" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="17" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="40" fillId="9" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="40" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="41" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -6706,31 +6669,7 @@
     <cellStyle name="Result" xfId="14" xr:uid="{6F03FC13-A797-4115-B488-D5132E8D2E66}"/>
     <cellStyle name="Result2" xfId="15" xr:uid="{8B643F58-BFEA-4FDF-8CA6-D5886F8338D7}"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-        <family val="2"/>
-      </font>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -8618,18 +8557,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="139" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -8746,18 +8685,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6C5642-BF97-4AFF-B370-04CC3D024494}">
-  <dimension ref="A1:AMJ50"/>
+  <dimension ref="A1:AMJ39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.25" style="22" customWidth="1"/>
+    <col min="1" max="1" width="10.25" style="21" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="4" customWidth="1"/>
     <col min="3" max="3" width="71.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="19" customWidth="1"/>
     <col min="5" max="5" width="1.625" style="4" customWidth="1"/>
     <col min="6" max="6" width="4.25" style="4" customWidth="1"/>
     <col min="7" max="7" width="49" style="4" bestFit="1" customWidth="1"/>
@@ -8769,38 +8708,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="F1" s="132" t="s">
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="F1" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
     </row>
     <row r="2" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="F2" s="134" t="s">
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="F2" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
     </row>
     <row r="3" spans="1:1024" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8821,20 +8760,20 @@
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="135" t="s">
+      <c r="H3" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="149"/>
+      <c r="L3" s="149"/>
     </row>
     <row r="4" spans="1:1024" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="129"/>
-      <c r="C4" s="129"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
       <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
@@ -8945,25 +8884,25 @@
       <c r="D7" s="13">
         <v>3</v>
       </c>
-      <c r="F7" s="163">
+      <c r="F7" s="126">
         <v>3</v>
       </c>
-      <c r="G7" s="164" t="s">
+      <c r="G7" s="127" t="s">
         <v>221</v>
       </c>
-      <c r="H7" s="165">
+      <c r="H7" s="128">
         <v>10</v>
       </c>
-      <c r="I7" s="165">
+      <c r="I7" s="128">
         <v>10</v>
       </c>
-      <c r="J7" s="165">
+      <c r="J7" s="128">
         <v>0</v>
       </c>
-      <c r="K7" s="165">
+      <c r="K7" s="128">
         <v>8</v>
       </c>
-      <c r="L7" s="166">
+      <c r="L7" s="129">
         <f>SUM(H7:K7)</f>
         <v>28</v>
       </c>
@@ -9032,11 +8971,11 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="140"/>
       <c r="D11" s="8">
         <f>SUM(D5:D10)</f>
         <v>25</v>
@@ -9119,7 +9058,7 @@
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="171" t="s">
+      <c r="C15" s="131" t="s">
         <v>222</v>
       </c>
       <c r="D15" s="13">
@@ -9140,8 +9079,8 @@
       <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="172" t="s">
-        <v>224</v>
+      <c r="C16" s="132" t="s">
+        <v>223</v>
       </c>
       <c r="D16" s="13">
         <v>6</v>
@@ -9161,8 +9100,8 @@
       <c r="B17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="170" t="s">
-        <v>225</v>
+      <c r="C17" s="130" t="s">
+        <v>224</v>
       </c>
       <c r="D17" s="13">
         <v>3</v>
@@ -9182,8 +9121,8 @@
       <c r="B18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="170" t="s">
-        <v>226</v>
+      <c r="C18" s="130" t="s">
+        <v>225</v>
       </c>
       <c r="D18" s="13">
         <v>6</v>
@@ -9196,270 +9135,211 @@
       <c r="AMI18"/>
       <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="171" t="s">
-        <v>223</v>
+      <c r="C19" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="D19" s="13">
-        <v>4</v>
-      </c>
-      <c r="AMD19"/>
-      <c r="AME19"/>
-      <c r="AMF19"/>
-      <c r="AMG19"/>
-      <c r="AMH19"/>
-      <c r="AMI19"/>
-      <c r="AMJ19"/>
-    </row>
-    <row r="20" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="172" t="s">
-        <v>227</v>
+      <c r="C20" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="D20" s="13">
-        <v>6</v>
-      </c>
-      <c r="AMD20"/>
-      <c r="AME20"/>
-      <c r="AMF20"/>
-      <c r="AMG20"/>
-      <c r="AMH20"/>
-      <c r="AMI20"/>
-      <c r="AMJ20"/>
-    </row>
-    <row r="21" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
-        <v>16</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="170" t="s">
-        <v>228</v>
-      </c>
-      <c r="D21" s="13">
-        <v>3</v>
-      </c>
-      <c r="AMD21"/>
-      <c r="AME21"/>
-      <c r="AMF21"/>
-      <c r="AMG21"/>
-      <c r="AMH21"/>
-      <c r="AMI21"/>
-      <c r="AMJ21"/>
-    </row>
-    <row r="22" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+    </row>
+    <row r="21" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="141" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="142"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="8">
+        <f>SUM(D12:D20)</f>
+        <v>57</v>
+      </c>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="170" t="s">
-        <v>229</v>
+        <v>37</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="D22" s="13">
-        <v>6</v>
-      </c>
-      <c r="AMD22"/>
-      <c r="AME22"/>
-      <c r="AMF22"/>
-      <c r="AMG22"/>
-      <c r="AMH22"/>
-      <c r="AMI22"/>
-      <c r="AMJ22"/>
+        <v>2</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
     </row>
     <row r="23" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D23" s="13">
-        <v>4</v>
-      </c>
-      <c r="AMD23"/>
-      <c r="AME23"/>
-      <c r="AMF23"/>
-      <c r="AMG23"/>
-      <c r="AMH23"/>
-      <c r="AMI23"/>
-      <c r="AMJ23"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>231</v>
+        <v>37</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>229</v>
       </c>
       <c r="D24" s="13">
-        <v>6</v>
-      </c>
-      <c r="AMD24"/>
-      <c r="AME24"/>
-      <c r="AMF24"/>
-      <c r="AMG24"/>
-      <c r="AMH24"/>
-      <c r="AMI24"/>
-      <c r="AMJ24"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="170" t="s">
-        <v>232</v>
+        <v>37</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>230</v>
       </c>
       <c r="D25" s="13">
-        <v>3</v>
-      </c>
-      <c r="AMD25"/>
-      <c r="AME25"/>
-      <c r="AMF25"/>
-      <c r="AMG25"/>
-      <c r="AMH25"/>
-      <c r="AMI25"/>
-      <c r="AMJ25"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
         <v>31</v>
       </c>
-      <c r="C26" s="170" t="s">
-        <v>233</v>
-      </c>
-      <c r="D26" s="13">
-        <v>6</v>
-      </c>
-      <c r="AMD26"/>
-      <c r="AME26"/>
-      <c r="AMF26"/>
-      <c r="AMG26"/>
-      <c r="AMH26"/>
-      <c r="AMI26"/>
-      <c r="AMJ26"/>
-    </row>
-    <row r="27" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A27" s="10">
-        <v>22</v>
-      </c>
       <c r="B27" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
       </c>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-    </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
-        <v>23</v>
-      </c>
-      <c r="B28" s="11" t="s">
+    </row>
+    <row r="28" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="140" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="140"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="8">
+        <f>SUM(D22:D27)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
         <v>31</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="13">
+      <c r="B29" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="13">
         <v>2</v>
       </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-    </row>
-    <row r="29" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="167" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="168"/>
-      <c r="C29" s="169"/>
-      <c r="D29" s="8">
-        <f>SUM(D12:D28)</f>
-        <v>95</v>
-      </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-    </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="D30" s="13">
-        <v>2</v>
-      </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>234</v>
+        <v>38</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="D31" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:1024" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>235</v>
+        <v>38</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="D32" s="13">
         <v>6</v>
@@ -9467,27 +9347,27 @@
     </row>
     <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>236</v>
+        <v>38</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D33" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>237</v>
+        <v>38</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="D34" s="13">
         <v>6</v>
@@ -9495,38 +9375,38 @@
     </row>
     <row r="35" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>238</v>
+        <v>38</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D35" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>239</v>
+        <v>38</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="D36" s="13">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
-        <v>30</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>35</v>
@@ -9535,170 +9415,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="10">
-        <v>31</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="129" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="129"/>
-      <c r="C39" s="129"/>
-      <c r="D39" s="8">
-        <f>SUM(D30:D38)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="10">
-        <v>31</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="10">
-        <v>32</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="10">
-        <v>33</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="10">
-        <v>34</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="10">
+    <row r="38" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="144"/>
+      <c r="B38" s="144"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="8">
+        <f>SUM(D29:D37)</f>
         <v>35</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="10">
-        <v>36</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="10">
-        <v>37</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="10">
-        <v>38</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="10">
-        <v>39</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="130"/>
-      <c r="B49" s="130"/>
-      <c r="C49" s="130"/>
-      <c r="D49" s="8">
-        <f>SUM(D40:D48)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="D50" s="23">
-        <f>SUM(D11,D29,D39,D49)</f>
-        <v>185</v>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D39" s="22">
+        <f>SUM(D11,D21,D28,D38)</f>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -9709,9 +9438,9 @@
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A38:C38"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="1.1437007874015752" bottom="1.1437007874015752" header="0.75000000000000011" footer="0.75000000000000011"/>
@@ -9733,47 +9462,47 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="24" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="23" customWidth="1"/>
     <col min="3" max="3" width="20.75" style="1" customWidth="1"/>
     <col min="4" max="1024" width="8.125" style="1" customWidth="1"/>
     <col min="1025" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="150" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
     </row>
     <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="26">
-        <f>Backlog_Produto!$D$50</f>
-        <v>185</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="25">
+        <f>Backlog_Produto!$D$39</f>
+        <v>147</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>0.4</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -9781,168 +9510,168 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <v>1</v>
       </c>
-      <c r="C6" s="29"/>
+      <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>20</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="30">
         <f>B6*B7*2</f>
         <v>40</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <f>B11/2</f>
-        <v>6.4749999999999996</v>
-      </c>
-      <c r="C9" s="32" t="s">
+        <v>5.1450000000000005</v>
+      </c>
+      <c r="C9" s="31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="32">
         <f>B4+(B4*B5)</f>
-        <v>259</v>
-      </c>
-      <c r="C10" s="34" t="s">
+        <v>205.8</v>
+      </c>
+      <c r="C10" s="33" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="30">
         <f>B10/B8*2</f>
-        <v>12.95</v>
-      </c>
-      <c r="C11" s="29" t="s">
+        <v>10.290000000000001</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="34">
         <f>B11/4</f>
-        <v>3.2374999999999998</v>
-      </c>
-      <c r="C12" s="25" t="s">
+        <v>2.5725000000000002</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="151" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
+      <c r="B14" s="151"/>
+      <c r="C14" s="151"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="35">
         <v>20</v>
       </c>
-      <c r="C15" s="37"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="37">
         <f>B10*B15</f>
-        <v>5180</v>
-      </c>
-      <c r="C16" s="37"/>
+        <v>4116</v>
+      </c>
+      <c r="C16" s="36"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>0.2</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="36"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="39">
+      <c r="B18" s="38">
         <f>B16*B17</f>
-        <v>1036</v>
-      </c>
-      <c r="C18" s="37"/>
+        <v>823.2</v>
+      </c>
+      <c r="C18" s="36"/>
     </row>
     <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="41">
+      <c r="B19" s="40">
         <f>B16+B18</f>
-        <v>6216</v>
-      </c>
-      <c r="C19" s="37"/>
+        <v>4939.2</v>
+      </c>
+      <c r="C19" s="36"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="27">
         <v>0.2</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="36"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="41">
         <f>B19*B20</f>
-        <v>1243.2</v>
-      </c>
-      <c r="C21" s="37"/>
+        <v>987.84</v>
+      </c>
+      <c r="C21" s="36"/>
     </row>
     <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="41">
+      <c r="B22" s="40">
         <f>B19+B21</f>
-        <v>7459.2</v>
-      </c>
-      <c r="C22" s="37"/>
+        <v>5927.04</v>
+      </c>
+      <c r="C22" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9967,335 +9696,335 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.125" style="71" customWidth="1"/>
+    <col min="1" max="1" width="6.125" style="70" customWidth="1"/>
     <col min="2" max="2" width="47.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="71" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="70" customWidth="1"/>
     <col min="4" max="6" width="13.125" style="4" customWidth="1"/>
     <col min="7" max="9" width="13" style="4" customWidth="1"/>
-    <col min="10" max="10" width="13" style="22" customWidth="1"/>
+    <col min="10" max="10" width="13" style="21" customWidth="1"/>
     <col min="11" max="11" width="14.75" style="4" customWidth="1"/>
     <col min="12" max="1024" width="8.5" style="4" customWidth="1"/>
     <col min="1025" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="155" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="155"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="43">
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="42">
         <f>Planejamento!$B$10</f>
-        <v>259</v>
-      </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="139" t="s">
+        <v>205.8</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="43"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="42"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="140" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="141" t="s">
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="158" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="50"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="47" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="52">
+      <c r="A5" s="51">
         <v>1</v>
       </c>
-      <c r="B5" s="173" t="s">
+      <c r="B5" s="133" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="174" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" s="174">
+      <c r="C5" s="134" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="134">
         <v>45904</v>
       </c>
-      <c r="E5" s="175">
+      <c r="E5" s="135">
         <v>25</v>
       </c>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="174" t="s">
-        <v>240</v>
-      </c>
-      <c r="H5" s="174">
+      <c r="G5" s="134" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="134">
         <v>45904</v>
       </c>
-      <c r="I5" s="54">
+      <c r="I5" s="53">
         <v>24</v>
       </c>
-      <c r="J5" s="55">
+      <c r="J5" s="54">
         <f>E5-I5</f>
         <v>1</v>
       </c>
-      <c r="K5" s="56" t="s">
-        <v>241</v>
+      <c r="K5" s="55" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="52">
+      <c r="A6" s="51">
         <v>2</v>
       </c>
-      <c r="B6" s="177" t="s">
+      <c r="B6" s="137" t="s">
         <v>219</v>
       </c>
-      <c r="C6" s="174">
+      <c r="C6" s="134">
         <v>45904</v>
       </c>
-      <c r="D6" s="174">
+      <c r="D6" s="134">
         <v>45932</v>
       </c>
-      <c r="E6" s="178">
+      <c r="E6" s="152">
         <v>125</v>
       </c>
-      <c r="F6" s="176" t="s">
+      <c r="F6" s="136" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="56"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="55"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="52">
+      <c r="A7" s="51">
         <v>3</v>
       </c>
-      <c r="B7" s="173" t="s">
+      <c r="B7" s="133" t="s">
         <v>220</v>
       </c>
-      <c r="C7" s="174">
+      <c r="C7" s="134">
         <v>45932</v>
       </c>
-      <c r="D7" s="174">
+      <c r="D7" s="134">
         <v>45946</v>
       </c>
-      <c r="E7" s="179"/>
-      <c r="F7" s="176" t="s">
+      <c r="E7" s="153"/>
+      <c r="F7" s="136" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="56"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="55"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="52">
+      <c r="A8" s="51">
         <v>4</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="C8" s="60">
+      <c r="C8" s="59">
         <v>45946</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="59">
         <v>45960</v>
       </c>
-      <c r="E8" s="180"/>
-      <c r="F8" s="176" t="s">
+      <c r="E8" s="154"/>
+      <c r="F8" s="136" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="64"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="63"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="52">
+      <c r="A9" s="51">
         <v>5</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="60">
+      <c r="C9" s="59">
         <v>45960</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="59">
         <v>45974</v>
       </c>
-      <c r="E9" s="61">
+      <c r="E9" s="60">
         <v>35</v>
       </c>
-      <c r="F9" s="176" t="s">
+      <c r="F9" s="136" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="64"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="63"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="52">
+      <c r="A10" s="51">
         <v>6</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="64"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="63"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
+      <c r="A11" s="51">
         <v>7</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="64"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="63"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="52">
+      <c r="A12" s="51">
         <v>8</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="64"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="52">
+      <c r="A13" s="51">
         <v>9</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="63"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="52">
+      <c r="A14" s="51">
         <v>10</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="63"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="65"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="68">
+      <c r="A15" s="64"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="67">
         <f>SUM(E5:E14)</f>
         <v>185</v>
       </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="68">
+      <c r="F15" s="65"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="67">
         <f>SUM(I5:I14)</f>
         <v>24</v>
       </c>
-      <c r="J15" s="70">
+      <c r="J15" s="69">
         <f>SUM(J5:J14)</f>
         <v>1</v>
       </c>
-      <c r="K15" s="69"/>
+      <c r="K15" s="68"/>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="J16" s="22"/>
+      <c r="J16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -10307,45 +10036,29 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:D14">
-    <cfRule type="expression" dxfId="13" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>OR($F5="Planned",$F5="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>$F5="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F14">
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>$F5="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>$F5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H14">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
-      <formula>OR($F6="Planned",$F6="Unplanned")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
-      <formula>$F6="Ongoing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="G5:H14">
+    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
       <formula>OR($F5="Planned",$F5="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
-      <formula>$F5="Ongoing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>OR($F5="Planned",$F5="Unplanned")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>$F5="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10364,618 +10077,618 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000B64FE-1B63-401C-B573-13BE1BFD24E2}">
   <dimension ref="A1:AMJ60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.625" style="73" customWidth="1"/>
-    <col min="2" max="2" width="35.625" style="73" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="73" customWidth="1"/>
-    <col min="4" max="4" width="13.25" style="73" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="73" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="73" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="73" customWidth="1"/>
-    <col min="8" max="9" width="12.25" style="73" customWidth="1"/>
-    <col min="10" max="10" width="24.25" style="73" customWidth="1"/>
-    <col min="11" max="11" width="27.875" style="73" customWidth="1"/>
-    <col min="12" max="12" width="8.5" style="73" customWidth="1"/>
-    <col min="13" max="14" width="20.5" style="73" customWidth="1"/>
-    <col min="15" max="256" width="8.5" style="73" customWidth="1"/>
-    <col min="257" max="258" width="6.5" style="73" customWidth="1"/>
-    <col min="259" max="259" width="13.875" style="73" customWidth="1"/>
-    <col min="260" max="260" width="9" style="73" customWidth="1"/>
-    <col min="261" max="261" width="13.5" style="73" customWidth="1"/>
-    <col min="262" max="262" width="10" style="73" customWidth="1"/>
-    <col min="263" max="263" width="12.25" style="73" customWidth="1"/>
-    <col min="264" max="264" width="5.875" style="73" customWidth="1"/>
-    <col min="265" max="265" width="24.25" style="73" customWidth="1"/>
-    <col min="266" max="266" width="32.5" style="73" customWidth="1"/>
-    <col min="267" max="267" width="17.625" style="73" customWidth="1"/>
-    <col min="268" max="268" width="8.5" style="73" customWidth="1"/>
-    <col min="269" max="270" width="20.5" style="73" customWidth="1"/>
-    <col min="271" max="512" width="8.5" style="73" customWidth="1"/>
-    <col min="513" max="514" width="6.5" style="73" customWidth="1"/>
-    <col min="515" max="515" width="13.875" style="73" customWidth="1"/>
-    <col min="516" max="516" width="9" style="73" customWidth="1"/>
-    <col min="517" max="517" width="13.5" style="73" customWidth="1"/>
-    <col min="518" max="518" width="10" style="73" customWidth="1"/>
-    <col min="519" max="519" width="12.25" style="73" customWidth="1"/>
-    <col min="520" max="520" width="5.875" style="73" customWidth="1"/>
-    <col min="521" max="521" width="24.25" style="73" customWidth="1"/>
-    <col min="522" max="522" width="32.5" style="73" customWidth="1"/>
-    <col min="523" max="523" width="17.625" style="73" customWidth="1"/>
-    <col min="524" max="524" width="8.5" style="73" customWidth="1"/>
-    <col min="525" max="526" width="20.5" style="73" customWidth="1"/>
-    <col min="527" max="768" width="8.5" style="73" customWidth="1"/>
-    <col min="769" max="770" width="6.5" style="73" customWidth="1"/>
-    <col min="771" max="771" width="13.875" style="73" customWidth="1"/>
-    <col min="772" max="772" width="9" style="73" customWidth="1"/>
-    <col min="773" max="773" width="13.5" style="73" customWidth="1"/>
-    <col min="774" max="774" width="10" style="73" customWidth="1"/>
-    <col min="775" max="775" width="12.25" style="73" customWidth="1"/>
-    <col min="776" max="776" width="5.875" style="73" customWidth="1"/>
-    <col min="777" max="777" width="24.25" style="73" customWidth="1"/>
-    <col min="778" max="778" width="32.5" style="73" customWidth="1"/>
-    <col min="779" max="779" width="17.625" style="73" customWidth="1"/>
-    <col min="780" max="780" width="8.5" style="73" customWidth="1"/>
-    <col min="781" max="782" width="20.5" style="73" customWidth="1"/>
-    <col min="783" max="1024" width="8.5" style="73" customWidth="1"/>
+    <col min="1" max="1" width="5.625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="35.625" style="72" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="72" customWidth="1"/>
+    <col min="4" max="4" width="13.25" style="72" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="72" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="72" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="72" customWidth="1"/>
+    <col min="8" max="9" width="12.25" style="72" customWidth="1"/>
+    <col min="10" max="10" width="24.25" style="72" customWidth="1"/>
+    <col min="11" max="11" width="27.875" style="72" customWidth="1"/>
+    <col min="12" max="12" width="8.5" style="72" customWidth="1"/>
+    <col min="13" max="14" width="20.5" style="72" customWidth="1"/>
+    <col min="15" max="256" width="8.5" style="72" customWidth="1"/>
+    <col min="257" max="258" width="6.5" style="72" customWidth="1"/>
+    <col min="259" max="259" width="13.875" style="72" customWidth="1"/>
+    <col min="260" max="260" width="9" style="72" customWidth="1"/>
+    <col min="261" max="261" width="13.5" style="72" customWidth="1"/>
+    <col min="262" max="262" width="10" style="72" customWidth="1"/>
+    <col min="263" max="263" width="12.25" style="72" customWidth="1"/>
+    <col min="264" max="264" width="5.875" style="72" customWidth="1"/>
+    <col min="265" max="265" width="24.25" style="72" customWidth="1"/>
+    <col min="266" max="266" width="32.5" style="72" customWidth="1"/>
+    <col min="267" max="267" width="17.625" style="72" customWidth="1"/>
+    <col min="268" max="268" width="8.5" style="72" customWidth="1"/>
+    <col min="269" max="270" width="20.5" style="72" customWidth="1"/>
+    <col min="271" max="512" width="8.5" style="72" customWidth="1"/>
+    <col min="513" max="514" width="6.5" style="72" customWidth="1"/>
+    <col min="515" max="515" width="13.875" style="72" customWidth="1"/>
+    <col min="516" max="516" width="9" style="72" customWidth="1"/>
+    <col min="517" max="517" width="13.5" style="72" customWidth="1"/>
+    <col min="518" max="518" width="10" style="72" customWidth="1"/>
+    <col min="519" max="519" width="12.25" style="72" customWidth="1"/>
+    <col min="520" max="520" width="5.875" style="72" customWidth="1"/>
+    <col min="521" max="521" width="24.25" style="72" customWidth="1"/>
+    <col min="522" max="522" width="32.5" style="72" customWidth="1"/>
+    <col min="523" max="523" width="17.625" style="72" customWidth="1"/>
+    <col min="524" max="524" width="8.5" style="72" customWidth="1"/>
+    <col min="525" max="526" width="20.5" style="72" customWidth="1"/>
+    <col min="527" max="768" width="8.5" style="72" customWidth="1"/>
+    <col min="769" max="770" width="6.5" style="72" customWidth="1"/>
+    <col min="771" max="771" width="13.875" style="72" customWidth="1"/>
+    <col min="772" max="772" width="9" style="72" customWidth="1"/>
+    <col min="773" max="773" width="13.5" style="72" customWidth="1"/>
+    <col min="774" max="774" width="10" style="72" customWidth="1"/>
+    <col min="775" max="775" width="12.25" style="72" customWidth="1"/>
+    <col min="776" max="776" width="5.875" style="72" customWidth="1"/>
+    <col min="777" max="777" width="24.25" style="72" customWidth="1"/>
+    <col min="778" max="778" width="32.5" style="72" customWidth="1"/>
+    <col min="779" max="779" width="17.625" style="72" customWidth="1"/>
+    <col min="780" max="780" width="8.5" style="72" customWidth="1"/>
+    <col min="781" max="782" width="20.5" style="72" customWidth="1"/>
+    <col min="783" max="1024" width="8.5" style="72" customWidth="1"/>
     <col min="1025" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="72" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="138" t="s">
+    <row r="1" spans="1:11" s="71" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="155" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="155"/>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="73" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="74" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="74" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="74" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="74" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="74" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="75" t="s">
+      <c r="D9" s="74" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="74" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="74" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="74" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="75" t="s">
+      <c r="D13" s="74" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="73" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="74" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="74" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="75" t="s">
+      <c r="D17" s="74" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="18" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="73" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="75" t="s">
+      <c r="D19" s="74" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="75" t="s">
+      <c r="D20" s="74" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="21" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="75" t="s">
+      <c r="D21" s="74" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="22" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="73" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="23" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="75" t="s">
+      <c r="D23" s="74" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="24" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="74" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="25" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="75" t="s">
+      <c r="D25" s="74" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="26" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="74" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="27" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="73" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="28" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D28" s="75" t="s">
+      <c r="D28" s="74" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="29" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D29" s="75" t="s">
+      <c r="D29" s="74" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="30" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="74" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="4:4" s="76" customFormat="1" ht="11.25" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D31" s="77" t="s">
+    <row r="31" spans="4:4" s="75" customFormat="1" ht="11.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="76" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="32" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D32" s="78" t="s">
+      <c r="D32" s="77" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="148" t="s">
+      <c r="D33" s="166" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="148"/>
+      <c r="E33" s="166"/>
     </row>
     <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D34" s="75">
+      <c r="D34" s="74">
         <v>4290</v>
       </c>
-      <c r="E34" s="75" t="s">
+      <c r="E34" s="74" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D35" s="75">
+      <c r="D35" s="74">
         <v>5082</v>
       </c>
-      <c r="E35" s="75" t="s">
+      <c r="E35" s="74" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D36" s="75">
+      <c r="D36" s="74">
         <v>4356</v>
       </c>
-      <c r="E36" s="75" t="s">
+      <c r="E36" s="74" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="22.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D37" s="75">
+      <c r="D37" s="74">
         <v>5929</v>
       </c>
-      <c r="E37" s="75" t="s">
+      <c r="E37" s="74" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D38" s="75">
+      <c r="D38" s="74">
         <v>5005</v>
       </c>
-      <c r="E38" s="75" t="s">
+      <c r="E38" s="74" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="D39" s="75">
+      <c r="D39" s="74">
         <v>4225</v>
       </c>
-      <c r="E39" s="75" t="s">
+      <c r="E39" s="74" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:11" s="72" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="149" t="s">
+    <row r="41" spans="1:11" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="167" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="149"/>
-      <c r="C41" s="149"/>
-      <c r="D41" s="149"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="149"/>
-      <c r="G41" s="149"/>
-      <c r="H41" s="149"/>
-      <c r="I41" s="149"/>
-      <c r="J41" s="149"/>
-      <c r="K41" s="149"/>
-    </row>
-    <row r="42" spans="1:11" s="72" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="150" t="s">
+      <c r="B41" s="167"/>
+      <c r="C41" s="167"/>
+      <c r="D41" s="167"/>
+      <c r="E41" s="167"/>
+      <c r="F41" s="167"/>
+      <c r="G41" s="167"/>
+      <c r="H41" s="167"/>
+      <c r="I41" s="167"/>
+      <c r="J41" s="167"/>
+      <c r="K41" s="167"/>
+    </row>
+    <row r="42" spans="1:11" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="150"/>
-      <c r="C42" s="150"/>
-      <c r="D42" s="150"/>
-      <c r="E42" s="150"/>
-      <c r="F42" s="150"/>
-      <c r="G42" s="150"/>
-      <c r="H42" s="150"/>
-      <c r="I42" s="150"/>
-      <c r="J42" s="150"/>
-      <c r="K42" s="150"/>
-    </row>
-    <row r="43" spans="1:11" s="72" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="151" t="s">
+      <c r="B42" s="168"/>
+      <c r="C42" s="168"/>
+      <c r="D42" s="168"/>
+      <c r="E42" s="168"/>
+      <c r="F42" s="168"/>
+      <c r="G42" s="168"/>
+      <c r="H42" s="168"/>
+      <c r="I42" s="168"/>
+      <c r="J42" s="168"/>
+      <c r="K42" s="168"/>
+    </row>
+    <row r="43" spans="1:11" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="169" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="151"/>
-      <c r="C43" s="151"/>
-      <c r="D43" s="151"/>
-      <c r="E43" s="151"/>
-      <c r="F43" s="151"/>
-      <c r="G43" s="151"/>
-      <c r="H43" s="151"/>
-      <c r="I43" s="151"/>
-      <c r="J43" s="151"/>
-      <c r="K43" s="151"/>
-    </row>
-    <row r="44" spans="1:11" s="72" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="152" t="s">
+      <c r="B43" s="169"/>
+      <c r="C43" s="169"/>
+      <c r="D43" s="169"/>
+      <c r="E43" s="169"/>
+      <c r="F43" s="169"/>
+      <c r="G43" s="169"/>
+      <c r="H43" s="169"/>
+      <c r="I43" s="169"/>
+      <c r="J43" s="169"/>
+      <c r="K43" s="169"/>
+    </row>
+    <row r="44" spans="1:11" s="71" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="165" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="152"/>
-      <c r="C44" s="152"/>
-      <c r="D44" s="152"/>
-      <c r="E44" s="152"/>
-      <c r="F44" s="152"/>
-      <c r="G44" s="152"/>
-      <c r="H44" s="152"/>
-      <c r="I44" s="152"/>
-      <c r="J44" s="152"/>
-      <c r="K44" s="152"/>
+      <c r="B44" s="165"/>
+      <c r="C44" s="165"/>
+      <c r="D44" s="165"/>
+      <c r="E44" s="165"/>
+      <c r="F44" s="165"/>
+      <c r="G44" s="165"/>
+      <c r="H44" s="165"/>
+      <c r="I44" s="165"/>
+      <c r="J44" s="165"/>
+      <c r="K44" s="165"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="144" t="s">
+      <c r="A46" s="161" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="144"/>
-      <c r="C46" s="144"/>
-      <c r="D46" s="144"/>
-      <c r="E46" s="144"/>
-      <c r="F46" s="144"/>
-      <c r="G46" s="144"/>
-      <c r="H46" s="144"/>
-      <c r="I46" s="144"/>
-      <c r="J46" s="144"/>
-      <c r="K46" s="144"/>
-    </row>
-    <row r="47" spans="1:11" s="81" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="79" t="s">
+      <c r="B46" s="161"/>
+      <c r="C46" s="161"/>
+      <c r="D46" s="161"/>
+      <c r="E46" s="161"/>
+      <c r="F46" s="161"/>
+      <c r="G46" s="161"/>
+      <c r="H46" s="161"/>
+      <c r="I46" s="161"/>
+      <c r="J46" s="161"/>
+      <c r="K46" s="161"/>
+    </row>
+    <row r="47" spans="1:11" s="80" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="80"/>
-      <c r="C47" s="145" t="s">
+      <c r="B47" s="79"/>
+      <c r="C47" s="162" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="145"/>
-      <c r="E47" s="145"/>
-      <c r="F47" s="145"/>
-      <c r="G47" s="145"/>
-      <c r="H47" s="145"/>
-      <c r="I47" s="145"/>
-      <c r="J47" s="145"/>
-      <c r="K47" s="145"/>
-    </row>
-    <row r="48" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="146"/>
-      <c r="B48" s="142" t="s">
+      <c r="D47" s="162"/>
+      <c r="E47" s="162"/>
+      <c r="F47" s="162"/>
+      <c r="G47" s="162"/>
+      <c r="H47" s="162"/>
+      <c r="I47" s="162"/>
+      <c r="J47" s="162"/>
+      <c r="K47" s="162"/>
+    </row>
+    <row r="48" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="163"/>
+      <c r="B48" s="159" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="142" t="s">
+      <c r="C48" s="159" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="142" t="s">
+      <c r="D48" s="159" t="s">
         <v>134</v>
       </c>
-      <c r="E48" s="142" t="s">
+      <c r="E48" s="159" t="s">
         <v>103</v>
       </c>
-      <c r="F48" s="142" t="s">
+      <c r="F48" s="159" t="s">
         <v>135</v>
       </c>
-      <c r="G48" s="142" t="s">
+      <c r="G48" s="159" t="s">
         <v>107</v>
       </c>
-      <c r="H48" s="147" t="s">
+      <c r="H48" s="164" t="s">
         <v>136</v>
       </c>
-      <c r="I48" s="147"/>
-      <c r="J48" s="147"/>
-      <c r="K48" s="147"/>
-    </row>
-    <row r="49" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="146"/>
-      <c r="B49" s="142"/>
-      <c r="C49" s="142"/>
-      <c r="D49" s="142"/>
-      <c r="E49" s="142"/>
-      <c r="F49" s="142"/>
-      <c r="G49" s="142"/>
-      <c r="H49" s="142" t="s">
+      <c r="I48" s="164"/>
+      <c r="J48" s="164"/>
+      <c r="K48" s="164"/>
+    </row>
+    <row r="49" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="163"/>
+      <c r="B49" s="159"/>
+      <c r="C49" s="159"/>
+      <c r="D49" s="159"/>
+      <c r="E49" s="159"/>
+      <c r="F49" s="159"/>
+      <c r="G49" s="159"/>
+      <c r="H49" s="159" t="s">
         <v>137</v>
       </c>
-      <c r="I49" s="142"/>
-      <c r="J49" s="82" t="s">
+      <c r="I49" s="159"/>
+      <c r="J49" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="K49" s="82" t="s">
+      <c r="K49" s="81" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="83" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="84">
+    <row r="50" spans="1:11" s="82" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="83">
         <v>1</v>
       </c>
-      <c r="B50" s="85" t="s">
+      <c r="B50" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="C50" s="86">
+      <c r="C50" s="85">
         <v>43891</v>
       </c>
-      <c r="D50" s="87" t="s">
+      <c r="D50" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="87" t="s">
+      <c r="E50" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="88" t="str">
+      <c r="F50" s="87" t="str">
         <f t="shared" ref="F50:F60" si="0">IF(OR((CODE($D50)*CODE($E50))=$D$36,(CODE($D50)*CODE($E50))=$D$35),$D$15,IF(OR((CODE($D50)*CODE($E50))=$D$34,(CODE($D50)*CODE($E50))=$D$37),$D$16,IF(OR((CODE($D50)*CODE($E50))=$D$38,(CODE($D50)*CODE($E50))=$D$39),$D$17,0)))</f>
         <v>Média</v>
       </c>
-      <c r="G50" s="87" t="s">
+      <c r="G50" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="H50" s="143"/>
-      <c r="I50" s="143"/>
-      <c r="J50" s="89"/>
-      <c r="K50" s="89" t="s">
+      <c r="H50" s="160"/>
+      <c r="I50" s="160"/>
+      <c r="J50" s="88"/>
+      <c r="K50" s="88" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="84"/>
-      <c r="B51" s="85"/>
-      <c r="C51" s="86"/>
-      <c r="D51" s="87" t="s">
+    <row r="51" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="83"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="85"/>
+      <c r="D51" s="86" t="s">
         <v>100</v>
       </c>
-      <c r="E51" s="87"/>
-      <c r="F51" s="88" t="e">
+      <c r="E51" s="86"/>
+      <c r="F51" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G51" s="87"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="91"/>
-      <c r="J51" s="89"/>
-      <c r="K51" s="89"/>
-    </row>
-    <row r="52" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="84"/>
-      <c r="B52" s="85"/>
-      <c r="C52" s="86"/>
-      <c r="D52" s="87"/>
-      <c r="E52" s="87"/>
-      <c r="F52" s="88" t="e">
+      <c r="G51" s="86"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="88"/>
+      <c r="K51" s="88"/>
+    </row>
+    <row r="52" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="83"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="86"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G52" s="87"/>
-      <c r="H52" s="90"/>
-      <c r="I52" s="91"/>
-      <c r="J52" s="89"/>
-      <c r="K52" s="89"/>
-    </row>
-    <row r="53" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="84"/>
-      <c r="B53" s="85"/>
-      <c r="C53" s="86"/>
-      <c r="D53" s="87"/>
-      <c r="E53" s="87"/>
-      <c r="F53" s="88" t="e">
+      <c r="G52" s="86"/>
+      <c r="H52" s="89"/>
+      <c r="I52" s="90"/>
+      <c r="J52" s="88"/>
+      <c r="K52" s="88"/>
+    </row>
+    <row r="53" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="83"/>
+      <c r="B53" s="84"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G53" s="87"/>
-      <c r="H53" s="90"/>
-      <c r="I53" s="91"/>
-      <c r="J53" s="89"/>
-      <c r="K53" s="89"/>
-    </row>
-    <row r="54" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="84"/>
-      <c r="B54" s="85"/>
-      <c r="C54" s="86"/>
-      <c r="D54" s="87"/>
-      <c r="E54" s="87"/>
-      <c r="F54" s="88" t="e">
+      <c r="G53" s="86"/>
+      <c r="H53" s="89"/>
+      <c r="I53" s="90"/>
+      <c r="J53" s="88"/>
+      <c r="K53" s="88"/>
+    </row>
+    <row r="54" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="83"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="86"/>
+      <c r="E54" s="86"/>
+      <c r="F54" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G54" s="87"/>
-      <c r="H54" s="90"/>
-      <c r="I54" s="91"/>
-      <c r="J54" s="89"/>
-      <c r="K54" s="89"/>
-    </row>
-    <row r="55" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="84"/>
-      <c r="B55" s="85"/>
-      <c r="C55" s="86"/>
-      <c r="D55" s="87"/>
-      <c r="E55" s="87"/>
-      <c r="F55" s="88" t="e">
+      <c r="G54" s="86"/>
+      <c r="H54" s="89"/>
+      <c r="I54" s="90"/>
+      <c r="J54" s="88"/>
+      <c r="K54" s="88"/>
+    </row>
+    <row r="55" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="83"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="86"/>
+      <c r="E55" s="86"/>
+      <c r="F55" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G55" s="87"/>
-      <c r="H55" s="90"/>
-      <c r="I55" s="91"/>
-      <c r="J55" s="89"/>
-      <c r="K55" s="89"/>
-    </row>
-    <row r="56" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="84"/>
-      <c r="B56" s="85"/>
-      <c r="C56" s="86"/>
-      <c r="D56" s="87"/>
-      <c r="E56" s="87"/>
-      <c r="F56" s="88" t="e">
+      <c r="G55" s="86"/>
+      <c r="H55" s="89"/>
+      <c r="I55" s="90"/>
+      <c r="J55" s="88"/>
+      <c r="K55" s="88"/>
+    </row>
+    <row r="56" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="83"/>
+      <c r="B56" s="84"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G56" s="87"/>
-      <c r="H56" s="90"/>
-      <c r="I56" s="91"/>
-      <c r="J56" s="89"/>
-      <c r="K56" s="89"/>
-    </row>
-    <row r="57" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="84"/>
-      <c r="B57" s="85"/>
-      <c r="C57" s="86"/>
-      <c r="D57" s="87"/>
-      <c r="E57" s="87"/>
-      <c r="F57" s="88" t="e">
+      <c r="G56" s="86"/>
+      <c r="H56" s="89"/>
+      <c r="I56" s="90"/>
+      <c r="J56" s="88"/>
+      <c r="K56" s="88"/>
+    </row>
+    <row r="57" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="83"/>
+      <c r="B57" s="84"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="86"/>
+      <c r="E57" s="86"/>
+      <c r="F57" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G57" s="87"/>
-      <c r="H57" s="90"/>
-      <c r="I57" s="91"/>
-      <c r="J57" s="89"/>
-      <c r="K57" s="89"/>
-    </row>
-    <row r="58" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="84"/>
-      <c r="B58" s="85"/>
-      <c r="C58" s="86"/>
-      <c r="D58" s="87"/>
-      <c r="E58" s="87"/>
-      <c r="F58" s="88" t="e">
+      <c r="G57" s="86"/>
+      <c r="H57" s="89"/>
+      <c r="I57" s="90"/>
+      <c r="J57" s="88"/>
+      <c r="K57" s="88"/>
+    </row>
+    <row r="58" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="83"/>
+      <c r="B58" s="84"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="86"/>
+      <c r="E58" s="86"/>
+      <c r="F58" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G58" s="87"/>
-      <c r="H58" s="90"/>
-      <c r="I58" s="91"/>
-      <c r="J58" s="89"/>
-      <c r="K58" s="89"/>
-    </row>
-    <row r="59" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="84"/>
-      <c r="B59" s="85"/>
-      <c r="C59" s="86"/>
-      <c r="D59" s="87"/>
-      <c r="E59" s="87"/>
-      <c r="F59" s="88" t="e">
+      <c r="G58" s="86"/>
+      <c r="H58" s="89"/>
+      <c r="I58" s="90"/>
+      <c r="J58" s="88"/>
+      <c r="K58" s="88"/>
+    </row>
+    <row r="59" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="83"/>
+      <c r="B59" s="84"/>
+      <c r="C59" s="85"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="86"/>
+      <c r="F59" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G59" s="87"/>
-      <c r="H59" s="143"/>
-      <c r="I59" s="143"/>
-      <c r="J59" s="89"/>
-      <c r="K59" s="89"/>
-    </row>
-    <row r="60" spans="1:11" s="83" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="84"/>
-      <c r="B60" s="85"/>
-      <c r="C60" s="86"/>
-      <c r="D60" s="87"/>
-      <c r="E60" s="87"/>
-      <c r="F60" s="88" t="e">
+      <c r="G59" s="86"/>
+      <c r="H59" s="160"/>
+      <c r="I59" s="160"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="88"/>
+    </row>
+    <row r="60" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="83"/>
+      <c r="B60" s="84"/>
+      <c r="C60" s="85"/>
+      <c r="D60" s="86"/>
+      <c r="E60" s="86"/>
+      <c r="F60" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G60" s="87"/>
-      <c r="H60" s="143"/>
-      <c r="I60" s="143"/>
-      <c r="J60" s="89"/>
-      <c r="K60" s="89"/>
+      <c r="G60" s="86"/>
+      <c r="H60" s="160"/>
+      <c r="I60" s="160"/>
+      <c r="J60" s="88"/>
+      <c r="K60" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -11001,13 +10714,13 @@
     <mergeCell ref="H48:K48"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
-    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
       <formula>$D$15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" stopIfTrue="1" operator="equal">
       <formula>$D$16</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" stopIfTrue="1" operator="equal">
       <formula>$D$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11060,432 +10773,432 @@
     <col min="1025" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="72" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="155" t="s">
+    <row r="1" spans="1:23" s="71" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="172" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
-      <c r="L1" s="155"/>
-      <c r="M1" s="155"/>
-      <c r="N1" s="155"/>
-    </row>
-    <row r="2" spans="1:23" s="92" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="156" t="s">
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="172"/>
+      <c r="J1" s="172"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
+    </row>
+    <row r="2" spans="1:23" s="91" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="173" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="156"/>
-      <c r="L2" s="156"/>
-      <c r="M2" s="156"/>
-      <c r="N2" s="156"/>
-    </row>
-    <row r="3" spans="1:23" s="92" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="157" t="s">
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
+      <c r="I2" s="173"/>
+      <c r="J2" s="173"/>
+      <c r="K2" s="173"/>
+      <c r="L2" s="173"/>
+      <c r="M2" s="173"/>
+      <c r="N2" s="173"/>
+    </row>
+    <row r="3" spans="1:23" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="157"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="157"/>
-      <c r="M3" s="157"/>
-      <c r="N3" s="157"/>
-    </row>
-    <row r="4" spans="1:23" s="92" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="158" t="s">
+      <c r="B3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="174"/>
+      <c r="J3" s="174"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="174"/>
+      <c r="M3" s="174"/>
+      <c r="N3" s="174"/>
+    </row>
+    <row r="4" spans="1:23" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="175" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="158"/>
-      <c r="C4" s="158"/>
-      <c r="D4" s="158"/>
-      <c r="E4" s="158"/>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="158"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="158"/>
-      <c r="M4" s="158"/>
-      <c r="N4" s="158"/>
-    </row>
-    <row r="5" spans="1:23" s="92" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="159" t="s">
+      <c r="B4" s="175"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="175"/>
+      <c r="E4" s="175"/>
+      <c r="F4" s="175"/>
+      <c r="G4" s="175"/>
+      <c r="H4" s="175"/>
+      <c r="I4" s="175"/>
+      <c r="J4" s="175"/>
+      <c r="K4" s="175"/>
+      <c r="L4" s="175"/>
+      <c r="M4" s="175"/>
+      <c r="N4" s="175"/>
+    </row>
+    <row r="5" spans="1:23" s="91" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="176" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="159"/>
-      <c r="C5" s="159"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="159"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
+      <c r="B5" s="176"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="176"/>
+      <c r="H5" s="176"/>
+      <c r="I5" s="176"/>
+      <c r="J5" s="176"/>
+      <c r="K5" s="176"/>
+      <c r="L5" s="176"/>
+      <c r="M5" s="176"/>
+      <c r="N5" s="176"/>
     </row>
     <row r="6" spans="1:23" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:23" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="153" t="s">
+      <c r="A7" s="170" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="153"/>
-      <c r="D7" s="153" t="s">
+      <c r="B7" s="170"/>
+      <c r="D7" s="170" t="s">
         <v>147</v>
       </c>
-      <c r="E7" s="153"/>
-      <c r="G7" s="153" t="s">
+      <c r="E7" s="170"/>
+      <c r="G7" s="170" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="153"/>
-      <c r="K7" s="153"/>
-      <c r="M7" s="153" t="s">
+      <c r="H7" s="170"/>
+      <c r="I7" s="170"/>
+      <c r="J7" s="170"/>
+      <c r="K7" s="170"/>
+      <c r="M7" s="170" t="s">
         <v>149</v>
       </c>
-      <c r="N7" s="153"/>
+      <c r="N7" s="170"/>
     </row>
     <row r="8" spans="1:23" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="94" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="95" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="96" t="s">
+      <c r="E8" s="95" t="s">
         <v>151</v>
       </c>
-      <c r="G8" s="95" t="s">
+      <c r="G8" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="94" t="s">
         <v>154</v>
       </c>
-      <c r="I8" s="95" t="s">
+      <c r="I8" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="K8" s="96" t="s">
+      <c r="K8" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="M8" s="96" t="s">
+      <c r="M8" s="95" t="s">
         <v>157</v>
       </c>
-      <c r="N8" s="96" t="s">
+      <c r="N8" s="95" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="92" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="93" t="s">
         <v>154</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="92" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="94" t="s">
+      <c r="E9" s="93" t="s">
         <v>154</v>
       </c>
-      <c r="G9" s="95" t="s">
+      <c r="G9" s="94" t="s">
         <v>161</v>
       </c>
-      <c r="H9" s="93">
+      <c r="H9" s="92">
         <v>2</v>
       </c>
-      <c r="I9" s="93">
+      <c r="I9" s="92">
         <v>0</v>
       </c>
-      <c r="J9" s="93">
+      <c r="J9" s="92">
         <v>0</v>
       </c>
-      <c r="K9" s="96">
+      <c r="K9" s="95">
         <f>(H9*4)+(I9*6)+(J9*8)</f>
         <v>8</v>
       </c>
-      <c r="M9" s="97" t="s">
+      <c r="M9" s="96" t="s">
         <v>162</v>
       </c>
-      <c r="N9" s="98"/>
+      <c r="N9" s="97"/>
     </row>
     <row r="10" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="92" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="93" t="s">
         <v>154</v>
       </c>
-      <c r="D10" s="93"/>
-      <c r="E10" s="94"/>
-      <c r="G10" s="95" t="s">
+      <c r="D10" s="92"/>
+      <c r="E10" s="93"/>
+      <c r="G10" s="94" t="s">
         <v>164</v>
       </c>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="96">
+      <c r="H10" s="92"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="95">
         <f>(H10*3)+(I10*4)+(J10*6)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="97" t="s">
+      <c r="M10" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="N10" s="98"/>
+      <c r="N10" s="97"/>
     </row>
     <row r="11" spans="1:23" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="93"/>
-      <c r="B11" s="94"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="94"/>
-      <c r="G11" s="153" t="s">
+      <c r="A11" s="92"/>
+      <c r="B11" s="93"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="93"/>
+      <c r="G11" s="170" t="s">
         <v>166</v>
       </c>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="153"/>
-      <c r="K11" s="153"/>
-      <c r="M11" s="97" t="s">
+      <c r="H11" s="170"/>
+      <c r="I11" s="170"/>
+      <c r="J11" s="170"/>
+      <c r="K11" s="170"/>
+      <c r="M11" s="96" t="s">
         <v>167</v>
       </c>
-      <c r="N11" s="98"/>
+      <c r="N11" s="97"/>
     </row>
     <row r="12" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A12" s="93"/>
-      <c r="B12" s="94"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="94"/>
-      <c r="G12" s="95" t="s">
+      <c r="A12" s="92"/>
+      <c r="B12" s="93"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="93"/>
+      <c r="G12" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="H12" s="95" t="s">
+      <c r="H12" s="94" t="s">
         <v>154</v>
       </c>
-      <c r="I12" s="95" t="s">
+      <c r="I12" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="J12" s="96" t="s">
+      <c r="J12" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="K12" s="96" t="s">
+      <c r="K12" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="M12" s="97" t="s">
+      <c r="M12" s="96" t="s">
         <v>168</v>
       </c>
-      <c r="N12" s="98"/>
+      <c r="N12" s="97"/>
     </row>
     <row r="13" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A13" s="93"/>
-      <c r="B13" s="94"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="94"/>
-      <c r="G13" s="95" t="s">
+      <c r="A13" s="92"/>
+      <c r="B13" s="93"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="93"/>
+      <c r="G13" s="94" t="s">
         <v>169</v>
       </c>
-      <c r="H13" s="93">
+      <c r="H13" s="92">
         <v>1</v>
       </c>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="96">
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="95">
         <f>(H13*3)+(I13*4)+(J13*6)</f>
         <v>3</v>
       </c>
-      <c r="M13" s="97" t="s">
+      <c r="M13" s="96" t="s">
         <v>170</v>
       </c>
-      <c r="N13" s="98"/>
+      <c r="N13" s="97"/>
       <c r="W13" s="4" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A14" s="93"/>
-      <c r="B14" s="94"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="94"/>
-      <c r="G14" s="95" t="s">
+      <c r="A14" s="92"/>
+      <c r="B14" s="93"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="93"/>
+      <c r="G14" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="96">
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="95">
         <f>(H14*4)+(I14*5)+(J14*7)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="97" t="s">
+      <c r="M14" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="N14" s="98"/>
+      <c r="N14" s="97"/>
     </row>
     <row r="15" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
-      <c r="B15" s="94"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="94"/>
-      <c r="G15" s="95" t="s">
+      <c r="A15" s="92"/>
+      <c r="B15" s="93"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="93"/>
+      <c r="G15" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="H15" s="93">
+      <c r="H15" s="92">
         <v>1</v>
       </c>
-      <c r="I15" s="93"/>
-      <c r="J15" s="93"/>
-      <c r="K15" s="96">
+      <c r="I15" s="92"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="95">
         <f>(H15*3)+(I15*4)+(J15*6)</f>
         <v>3</v>
       </c>
-      <c r="M15" s="97" t="s">
+      <c r="M15" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="N15" s="98"/>
+      <c r="N15" s="97"/>
     </row>
     <row r="16" spans="1:23" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="93"/>
-      <c r="B16" s="94"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="94"/>
-      <c r="G16" s="154" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="93"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="93"/>
+      <c r="G16" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="99">
+      <c r="H16" s="171"/>
+      <c r="I16" s="171"/>
+      <c r="J16" s="171"/>
+      <c r="K16" s="98">
         <f>SUM(K9,K10,K13,K14,K15)</f>
         <v>14</v>
       </c>
-      <c r="M16" s="97" t="s">
+      <c r="M16" s="96" t="s">
         <v>177</v>
       </c>
-      <c r="N16" s="98"/>
+      <c r="N16" s="97"/>
     </row>
     <row r="17" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A17" s="93"/>
-      <c r="B17" s="94"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="94"/>
-      <c r="M17" s="97" t="s">
+      <c r="A17" s="92"/>
+      <c r="B17" s="93"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="93"/>
+      <c r="M17" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="N17" s="98"/>
+      <c r="N17" s="97"/>
     </row>
     <row r="18" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A18" s="93"/>
-      <c r="B18" s="94"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="94"/>
-      <c r="M18" s="97" t="s">
+      <c r="A18" s="92"/>
+      <c r="B18" s="93"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="93"/>
+      <c r="M18" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N18" s="98"/>
+      <c r="N18" s="97"/>
     </row>
     <row r="19" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A19" s="93"/>
-      <c r="B19" s="94"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="94"/>
-      <c r="M19" s="97" t="s">
+      <c r="A19" s="92"/>
+      <c r="B19" s="93"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="93"/>
+      <c r="M19" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="N19" s="98"/>
+      <c r="N19" s="97"/>
     </row>
     <row r="20" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
-      <c r="B20" s="94"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="94"/>
-      <c r="M20" s="97" t="s">
+      <c r="A20" s="92"/>
+      <c r="B20" s="93"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="93"/>
+      <c r="M20" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="N20" s="98"/>
+      <c r="N20" s="97"/>
     </row>
     <row r="21" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="M21" s="97" t="s">
+      <c r="M21" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="N21" s="98"/>
+      <c r="N21" s="97"/>
     </row>
     <row r="22" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="M22" s="97" t="s">
+      <c r="M22" s="96" t="s">
         <v>183</v>
       </c>
-      <c r="N22" s="98"/>
+      <c r="N22" s="97"/>
     </row>
     <row r="23" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="M23" s="100" t="s">
+      <c r="M23" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="N23" s="101">
+      <c r="N23" s="100">
         <f>SUM(N9:N22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M24" s="100" t="s">
+      <c r="M24" s="99" t="s">
         <v>185</v>
       </c>
-      <c r="N24" s="99">
+      <c r="N24" s="98">
         <f>(N23*0.01)+0.65</f>
         <v>0.65</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M25" s="100" t="s">
+      <c r="M25" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="N25" s="102">
+      <c r="N25" s="101">
         <f>K16*N24</f>
         <v>9.1</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M26" s="100" t="s">
+      <c r="M26" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="N26" s="103">
+      <c r="N26" s="102">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="M27" s="104" t="s">
+      <c r="M27" s="103" t="s">
         <v>188</v>
       </c>
-      <c r="N27" s="105">
+      <c r="N27" s="104">
         <f>N25*N26</f>
         <v>172.9</v>
       </c>
@@ -11531,7 +11244,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="23" customWidth="1"/>
     <col min="3" max="3" width="12.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="1.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.875" style="1" customWidth="1"/>
@@ -11549,690 +11262,690 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
-      <c r="L1" s="155"/>
-      <c r="M1" s="155"/>
-      <c r="N1" s="155"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="172"/>
+      <c r="J1" s="172"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="178" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="E3" s="161" t="s">
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="E3" s="178" t="s">
         <v>189</v>
       </c>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
-      <c r="L3" s="161"/>
-      <c r="M3" s="161"/>
-      <c r="N3" s="161"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="178"/>
+      <c r="I3" s="178"/>
+      <c r="J3" s="178"/>
+      <c r="K3" s="178"/>
+      <c r="L3" s="178"/>
+      <c r="M3" s="178"/>
+      <c r="N3" s="178"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="105" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="107">
+      <c r="B4" s="106">
         <f>'#Estimativa-APF#'!$N$27</f>
         <v>172.9</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="162" t="s">
+      <c r="E4" s="179" t="s">
         <v>191</v>
       </c>
-      <c r="F4" s="160" t="s">
+      <c r="F4" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160" t="s">
+      <c r="G4" s="177"/>
+      <c r="H4" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160" t="s">
+      <c r="I4" s="177"/>
+      <c r="J4" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="160"/>
-      <c r="L4" s="160" t="s">
+      <c r="K4" s="177"/>
+      <c r="L4" s="177" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="160"/>
-      <c r="N4" s="108"/>
+      <c r="M4" s="177"/>
+      <c r="N4" s="107"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>0</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="E5" s="162"/>
-      <c r="F5" s="160" t="s">
+      <c r="E5" s="179"/>
+      <c r="F5" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160" t="s">
+      <c r="G5" s="177"/>
+      <c r="H5" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="160"/>
-      <c r="J5" s="160" t="s">
+      <c r="I5" s="177"/>
+      <c r="J5" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="160"/>
-      <c r="L5" s="160" t="s">
+      <c r="K5" s="177"/>
+      <c r="L5" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="160"/>
-      <c r="N5" s="40" t="s">
+      <c r="M5" s="177"/>
+      <c r="N5" s="39" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="108" t="s">
         <v>194</v>
       </c>
-      <c r="B6" s="110">
+      <c r="B6" s="109">
         <f>B4+(B4*B5)</f>
         <v>172.9</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="162"/>
-      <c r="F6" s="111">
+      <c r="E6" s="179"/>
+      <c r="F6" s="110">
         <f>B6*G6</f>
         <v>8.6450000000000014</v>
       </c>
-      <c r="G6" s="112">
+      <c r="G6" s="111">
         <v>0.05</v>
       </c>
-      <c r="H6" s="111">
+      <c r="H6" s="110">
         <f>B4*I6</f>
         <v>34.580000000000005</v>
       </c>
-      <c r="I6" s="112">
+      <c r="I6" s="111">
         <v>0.2</v>
       </c>
-      <c r="J6" s="111">
+      <c r="J6" s="110">
         <f>B4*K6</f>
         <v>112.38500000000001</v>
       </c>
-      <c r="K6" s="112">
+      <c r="K6" s="111">
         <v>0.65</v>
       </c>
-      <c r="L6" s="111">
+      <c r="L6" s="110">
         <f>B4*M6</f>
         <v>17.290000000000003</v>
       </c>
-      <c r="M6" s="112">
+      <c r="M6" s="111">
         <v>0.1</v>
       </c>
-      <c r="N6" s="111"/>
+      <c r="N6" s="110"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>1</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="E7" s="113" t="s">
+      <c r="C7" s="28"/>
+      <c r="E7" s="112" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="111">
+      <c r="F7" s="110">
         <f>F6*G7</f>
         <v>4.7547500000000014</v>
       </c>
-      <c r="G7" s="112">
+      <c r="G7" s="111">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H7" s="111">
+      <c r="H7" s="110">
         <f>H6*I7</f>
         <v>10.374000000000001</v>
       </c>
-      <c r="I7" s="112">
+      <c r="I7" s="111">
         <v>0.3</v>
       </c>
-      <c r="J7" s="111">
+      <c r="J7" s="110">
         <f>J6*K7</f>
         <v>13.4862</v>
       </c>
-      <c r="K7" s="112">
+      <c r="K7" s="111">
         <v>0.12</v>
       </c>
-      <c r="L7" s="111">
+      <c r="L7" s="110">
         <f>L6*M7</f>
         <v>0.86450000000000016</v>
       </c>
-      <c r="M7" s="112">
+      <c r="M7" s="111">
         <v>0.05</v>
       </c>
-      <c r="N7" s="114">
+      <c r="N7" s="113">
         <f>SUM(F7,H7,J7,L7)</f>
         <v>29.47945</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="29">
         <v>40</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="E8" s="113" t="s">
+      <c r="E8" s="112" t="s">
         <v>199</v>
       </c>
-      <c r="F8" s="111">
+      <c r="F8" s="110">
         <f>F6*G8</f>
         <v>1.2967500000000001</v>
       </c>
-      <c r="G8" s="112">
+      <c r="G8" s="111">
         <v>0.15</v>
       </c>
-      <c r="H8" s="111">
+      <c r="H8" s="110">
         <f>H6*I8</f>
         <v>6.9160000000000013</v>
       </c>
-      <c r="I8" s="112">
+      <c r="I8" s="111">
         <v>0.2</v>
       </c>
-      <c r="J8" s="111">
+      <c r="J8" s="110">
         <f>J6*K8</f>
         <v>11.238500000000002</v>
       </c>
-      <c r="K8" s="112">
+      <c r="K8" s="111">
         <v>0.1</v>
       </c>
-      <c r="L8" s="111">
+      <c r="L8" s="110">
         <f>L6*M8</f>
         <v>0.86450000000000016</v>
       </c>
-      <c r="M8" s="112">
+      <c r="M8" s="111">
         <v>0.05</v>
       </c>
-      <c r="N8" s="114">
+      <c r="N8" s="113">
         <f>SUM(F8,H8,J8,L8)</f>
         <v>20.315750000000001</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="29">
         <v>2</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="113" t="s">
+      <c r="E9" s="112" t="s">
         <v>201</v>
       </c>
-      <c r="F9" s="111">
+      <c r="F9" s="110">
         <f>F6*G9</f>
         <v>0.17290000000000003</v>
       </c>
-      <c r="G9" s="112">
+      <c r="G9" s="111">
         <v>0.02</v>
       </c>
-      <c r="H9" s="111">
+      <c r="H9" s="110">
         <f>H6*I9</f>
         <v>6.9160000000000013</v>
       </c>
-      <c r="I9" s="112">
+      <c r="I9" s="111">
         <v>0.2</v>
       </c>
-      <c r="J9" s="111">
+      <c r="J9" s="110">
         <f>J6*K9</f>
         <v>44.954000000000008</v>
       </c>
-      <c r="K9" s="112">
+      <c r="K9" s="111">
         <v>0.4</v>
       </c>
-      <c r="L9" s="111">
+      <c r="L9" s="110">
         <f>L6*M9</f>
         <v>2.5935000000000001</v>
       </c>
-      <c r="M9" s="112">
+      <c r="M9" s="111">
         <v>0.15</v>
       </c>
-      <c r="N9" s="114">
+      <c r="N9" s="113">
         <f>SUM(F9,H9,J9,L9)</f>
         <v>54.636400000000009</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="114" t="s">
         <v>202</v>
       </c>
-      <c r="B10" s="116">
+      <c r="B10" s="115">
         <f>(B7*B8)*B9</f>
         <v>80</v>
       </c>
-      <c r="C10" s="115" t="s">
+      <c r="C10" s="114" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="113" t="s">
+      <c r="E10" s="112" t="s">
         <v>203</v>
       </c>
-      <c r="F10" s="111">
+      <c r="F10" s="110">
         <f>F6*G10</f>
         <v>0.43225000000000008</v>
       </c>
-      <c r="G10" s="112">
+      <c r="G10" s="111">
         <v>0.05</v>
       </c>
-      <c r="H10" s="111">
+      <c r="H10" s="110">
         <f>H6*I10</f>
         <v>2.7664000000000004</v>
       </c>
-      <c r="I10" s="112">
+      <c r="I10" s="111">
         <v>0.08</v>
       </c>
-      <c r="J10" s="111">
+      <c r="J10" s="110">
         <f>J6*K10</f>
         <v>11.238500000000002</v>
       </c>
-      <c r="K10" s="112">
+      <c r="K10" s="111">
         <v>0.1</v>
       </c>
-      <c r="L10" s="111">
+      <c r="L10" s="110">
         <f>L6*M10</f>
         <v>1.7290000000000003</v>
       </c>
-      <c r="M10" s="112">
+      <c r="M10" s="111">
         <v>0.1</v>
       </c>
-      <c r="N10" s="114">
+      <c r="N10" s="113">
         <f>SUM(F10,H10,J10,L10)</f>
         <v>16.166150000000002</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="105" t="s">
         <v>204</v>
       </c>
-      <c r="B11" s="117">
+      <c r="B11" s="116">
         <f>B6/B10*2</f>
         <v>4.3224999999999998</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="112" t="s">
         <v>205</v>
       </c>
-      <c r="F11" s="111">
+      <c r="F11" s="110">
         <f>F6*G11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="112">
+      <c r="G11" s="111">
         <v>0</v>
       </c>
-      <c r="H11" s="111">
+      <c r="H11" s="110">
         <f>H6*I11</f>
         <v>0.6916000000000001</v>
       </c>
-      <c r="I11" s="112">
+      <c r="I11" s="111">
         <v>0.02</v>
       </c>
-      <c r="J11" s="111">
+      <c r="J11" s="110">
         <f>J6*K11</f>
         <v>5.619250000000001</v>
       </c>
-      <c r="K11" s="112">
+      <c r="K11" s="111">
         <v>0.05</v>
       </c>
-      <c r="L11" s="111">
+      <c r="L11" s="110">
         <f>L6*M11</f>
         <v>1.7290000000000003</v>
       </c>
-      <c r="M11" s="112">
+      <c r="M11" s="111">
         <v>0.1</v>
       </c>
-      <c r="N11" s="114">
+      <c r="N11" s="113">
         <f>SUM(F11,H11,J11,L11)</f>
         <v>8.0398500000000013</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="B12" s="117">
+      <c r="B12" s="116">
         <f>B11/4</f>
         <v>1.0806249999999999</v>
       </c>
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="118" t="s">
+      <c r="E12" s="117" t="s">
         <v>207</v>
       </c>
-      <c r="F12" s="119">
+      <c r="F12" s="118">
         <f t="shared" ref="F12:M12" si="0">SUM(F7:F11)</f>
         <v>6.6566500000000017</v>
       </c>
-      <c r="G12" s="120">
+      <c r="G12" s="119">
         <f t="shared" si="0"/>
         <v>0.77000000000000013</v>
       </c>
-      <c r="H12" s="119">
+      <c r="H12" s="118">
         <f t="shared" si="0"/>
         <v>27.664000000000005</v>
       </c>
-      <c r="I12" s="120">
+      <c r="I12" s="119">
         <f t="shared" si="0"/>
         <v>0.79999999999999993</v>
       </c>
-      <c r="J12" s="119">
+      <c r="J12" s="118">
         <f t="shared" si="0"/>
         <v>86.536450000000002</v>
       </c>
-      <c r="K12" s="120">
+      <c r="K12" s="119">
         <f t="shared" si="0"/>
         <v>0.77</v>
       </c>
-      <c r="L12" s="119">
+      <c r="L12" s="118">
         <f t="shared" si="0"/>
         <v>7.7805000000000009</v>
       </c>
-      <c r="M12" s="120">
+      <c r="M12" s="119">
         <f t="shared" si="0"/>
         <v>0.44999999999999996</v>
       </c>
-      <c r="N12" s="118"/>
+      <c r="N12" s="117"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="115" t="s">
+      <c r="A13" s="114" t="s">
         <v>208</v>
       </c>
-      <c r="B13" s="121">
+      <c r="B13" s="120">
         <f>B11/B9</f>
         <v>2.1612499999999999</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="114" t="s">
         <v>209</v>
       </c>
-      <c r="E13" s="113" t="s">
+      <c r="E13" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="F13" s="111">
+      <c r="F13" s="110">
         <f>F6*G13</f>
         <v>0.25935000000000002</v>
       </c>
-      <c r="G13" s="112">
+      <c r="G13" s="111">
         <v>0.03</v>
       </c>
-      <c r="H13" s="111">
+      <c r="H13" s="110">
         <f>H6*I13</f>
         <v>2.7664000000000004</v>
       </c>
-      <c r="I13" s="112">
+      <c r="I13" s="111">
         <v>0.08</v>
       </c>
-      <c r="J13" s="111">
+      <c r="J13" s="110">
         <f>J6*K13</f>
         <v>14.610050000000001</v>
       </c>
-      <c r="K13" s="112">
+      <c r="K13" s="111">
         <v>0.13</v>
       </c>
-      <c r="L13" s="111">
+      <c r="L13" s="110">
         <f>L6*M13</f>
         <v>5.1870000000000003</v>
       </c>
-      <c r="M13" s="112">
+      <c r="M13" s="111">
         <v>0.3</v>
       </c>
-      <c r="N13" s="114">
+      <c r="N13" s="113">
         <f>SUM(F13,H13,J13,L13)</f>
         <v>22.822800000000004</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E14" s="113" t="s">
+      <c r="E14" s="112" t="s">
         <v>211</v>
       </c>
-      <c r="F14" s="111">
+      <c r="F14" s="110">
         <f>F6*G14</f>
         <v>1.7290000000000003</v>
       </c>
-      <c r="G14" s="112">
+      <c r="G14" s="111">
         <v>0.2</v>
       </c>
-      <c r="H14" s="111">
+      <c r="H14" s="110">
         <f>H6*I14</f>
         <v>4.1496000000000004</v>
       </c>
-      <c r="I14" s="112">
+      <c r="I14" s="111">
         <v>0.12</v>
       </c>
-      <c r="J14" s="111">
+      <c r="J14" s="110">
         <f>J6*K14</f>
         <v>11.238500000000002</v>
       </c>
-      <c r="K14" s="112">
+      <c r="K14" s="111">
         <v>0.1</v>
       </c>
-      <c r="L14" s="111">
+      <c r="L14" s="110">
         <f>L6*M14</f>
         <v>4.3225000000000007</v>
       </c>
-      <c r="M14" s="112">
+      <c r="M14" s="111">
         <v>0.25</v>
       </c>
-      <c r="N14" s="114">
+      <c r="N14" s="113">
         <f>SUM(F14,H14,J14,L14)</f>
         <v>21.439600000000002</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E15" s="118" t="s">
+      <c r="E15" s="117" t="s">
         <v>212</v>
       </c>
-      <c r="F15" s="119">
+      <c r="F15" s="118">
         <f t="shared" ref="F15:M15" si="1">SUM(F13:F14)</f>
         <v>1.9883500000000003</v>
       </c>
-      <c r="G15" s="120">
+      <c r="G15" s="119">
         <f t="shared" si="1"/>
         <v>0.23</v>
       </c>
-      <c r="H15" s="119">
+      <c r="H15" s="118">
         <f t="shared" si="1"/>
         <v>6.9160000000000004</v>
       </c>
-      <c r="I15" s="120">
+      <c r="I15" s="119">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="J15" s="119">
+      <c r="J15" s="118">
         <f t="shared" si="1"/>
         <v>25.848550000000003</v>
       </c>
-      <c r="K15" s="120">
+      <c r="K15" s="119">
         <f t="shared" si="1"/>
         <v>0.23</v>
       </c>
-      <c r="L15" s="119">
+      <c r="L15" s="118">
         <f t="shared" si="1"/>
         <v>9.509500000000001</v>
       </c>
-      <c r="M15" s="120">
+      <c r="M15" s="119">
         <f t="shared" si="1"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="N15" s="118"/>
+      <c r="N15" s="117"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="161" t="s">
+      <c r="A16" s="178" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="161"/>
-      <c r="C16" s="161"/>
-      <c r="E16" s="40" t="s">
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="E16" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="F16" s="122">
+      <c r="F16" s="121">
         <f t="shared" ref="F16:M16" si="2">F12+F15</f>
         <v>8.6450000000000014</v>
       </c>
-      <c r="G16" s="123">
+      <c r="G16" s="122">
         <f t="shared" si="2"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="H16" s="122">
+      <c r="H16" s="121">
         <f t="shared" si="2"/>
         <v>34.580000000000005</v>
       </c>
-      <c r="I16" s="123">
+      <c r="I16" s="122">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J16" s="122">
+      <c r="J16" s="121">
         <f t="shared" si="2"/>
         <v>112.38500000000001</v>
       </c>
-      <c r="K16" s="123">
+      <c r="K16" s="122">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L16" s="122">
+      <c r="L16" s="121">
         <f t="shared" si="2"/>
         <v>17.290000000000003</v>
       </c>
-      <c r="M16" s="123">
+      <c r="M16" s="122">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N16" s="124">
+      <c r="N16" s="123">
         <f>SUM(N7:N11,N13,N14)</f>
         <v>172.90000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="125">
+      <c r="B17" s="124">
         <v>20</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="N17" s="69"/>
+      <c r="C17" s="36"/>
+      <c r="N17" s="68"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="38">
+      <c r="B18" s="37">
         <f>B6*B17</f>
         <v>3458</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="L18" s="69"/>
-      <c r="N18" s="69"/>
+      <c r="C18" s="36"/>
+      <c r="L18" s="68"/>
+      <c r="N18" s="68"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="27">
         <v>0</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="N19" s="69"/>
+      <c r="C19" s="36"/>
+      <c r="N19" s="68"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="39">
+      <c r="B20" s="38">
         <f>B18*B19</f>
         <v>0</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="L20" s="69"/>
-      <c r="N20" s="69"/>
+      <c r="C20" s="36"/>
+      <c r="L20" s="68"/>
+      <c r="N20" s="68"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="B21" s="126">
+      <c r="B21" s="125">
         <f>B18+B20</f>
         <v>3458</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="N21" s="69"/>
+      <c r="C21" s="36"/>
+      <c r="N21" s="68"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="27">
         <v>0.2</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="J22" s="69"/>
+      <c r="C22" s="36"/>
+      <c r="J22" s="68"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="41">
         <f>B21*B22</f>
         <v>691.6</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="36"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="B24" s="126">
+      <c r="B24" s="125">
         <f>B21+B23</f>
         <v>4149.6000000000004</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="36"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J26" s="69"/>
+      <c r="J26" s="68"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J27" s="69"/>
+      <c r="J27" s="68"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N28" s="69"/>
+      <c r="N28" s="68"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N29" s="69"/>
+      <c r="N29" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Revisar os documentos faltandos.
</commit_message>
<xml_diff>
--- a/6.Gerenciamento de Projeto/SYLF - Planejamento e Controle do Projeto.xlsx
+++ b/6.Gerenciamento de Projeto/SYLF - Planejamento e Controle do Projeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\School\6 semestre\ESO\SYLF\6.Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E1C61E-F125-45D0-AB70-1D3DA1CA4BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567BFDEA-D5D0-483A-8A76-55BBAC6CBE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{31237A52-FFD1-4E1D-B5BB-391D11929C61}"/>
   </bookViews>
@@ -6529,6 +6529,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="7" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -6549,18 +6561,6 @@
     <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6591,6 +6591,21 @@
     <xf numFmtId="164" fontId="28" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="31" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="14" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="32" fillId="15" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6604,21 +6619,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="32" fillId="15" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="14" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8687,7 +8687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6C5642-BF97-4AFF-B370-04CC3D024494}">
   <dimension ref="A1:AMJ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -8708,38 +8708,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="F1" s="146" t="s">
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="F1" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
+      <c r="L1" s="140"/>
     </row>
     <row r="2" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="F2" s="148" t="s">
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="F2" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
     </row>
     <row r="3" spans="1:1024" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8760,20 +8760,20 @@
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="149" t="s">
+      <c r="H3" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="149"/>
-      <c r="J3" s="149"/>
-      <c r="K3" s="149"/>
-      <c r="L3" s="149"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
     </row>
     <row r="4" spans="1:1024" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="140"/>
-      <c r="C4" s="140"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="144"/>
       <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
@@ -8971,11 +8971,11 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="140" t="s">
+      <c r="A11" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="140"/>
-      <c r="C11" s="140"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="144"/>
       <c r="D11" s="8">
         <f>SUM(D5:D10)</f>
         <v>25</v>
@@ -9174,11 +9174,11 @@
       <c r="L20" s="19"/>
     </row>
     <row r="21" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="141" t="s">
+      <c r="A21" s="145" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="142"/>
-      <c r="C21" s="143"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="147"/>
       <c r="D21" s="8">
         <f>SUM(D12:D20)</f>
         <v>57</v>
@@ -9279,11 +9279,11 @@
       </c>
     </row>
     <row r="28" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="140" t="s">
+      <c r="A28" s="144" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="140"/>
-      <c r="C28" s="140"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
       <c r="D28" s="8">
         <f>SUM(D22:D27)</f>
         <v>30</v>
@@ -9416,9 +9416,9 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="144"/>
-      <c r="B38" s="144"/>
-      <c r="C38" s="144"/>
+      <c r="A38" s="148"/>
+      <c r="B38" s="148"/>
+      <c r="C38" s="148"/>
       <c r="D38" s="8">
         <f>SUM(D29:D37)</f>
         <v>35</v>
@@ -9432,16 +9432,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:L1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:L2"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="1.1437007874015752" bottom="1.1437007874015752" header="0.75000000000000011" footer="0.75000000000000011"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -10305,10 +10305,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="166" t="s">
+      <c r="D33" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="166"/>
+      <c r="E33" s="160"/>
     </row>
     <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="D34" s="74">
@@ -10360,137 +10360,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:11" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="167" t="s">
+      <c r="A41" s="161" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="167"/>
-      <c r="C41" s="167"/>
-      <c r="D41" s="167"/>
-      <c r="E41" s="167"/>
-      <c r="F41" s="167"/>
-      <c r="G41" s="167"/>
-      <c r="H41" s="167"/>
-      <c r="I41" s="167"/>
-      <c r="J41" s="167"/>
-      <c r="K41" s="167"/>
+      <c r="B41" s="161"/>
+      <c r="C41" s="161"/>
+      <c r="D41" s="161"/>
+      <c r="E41" s="161"/>
+      <c r="F41" s="161"/>
+      <c r="G41" s="161"/>
+      <c r="H41" s="161"/>
+      <c r="I41" s="161"/>
+      <c r="J41" s="161"/>
+      <c r="K41" s="161"/>
     </row>
     <row r="42" spans="1:11" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="168" t="s">
+      <c r="A42" s="162" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="168"/>
-      <c r="C42" s="168"/>
-      <c r="D42" s="168"/>
-      <c r="E42" s="168"/>
-      <c r="F42" s="168"/>
-      <c r="G42" s="168"/>
-      <c r="H42" s="168"/>
-      <c r="I42" s="168"/>
-      <c r="J42" s="168"/>
-      <c r="K42" s="168"/>
+      <c r="B42" s="162"/>
+      <c r="C42" s="162"/>
+      <c r="D42" s="162"/>
+      <c r="E42" s="162"/>
+      <c r="F42" s="162"/>
+      <c r="G42" s="162"/>
+      <c r="H42" s="162"/>
+      <c r="I42" s="162"/>
+      <c r="J42" s="162"/>
+      <c r="K42" s="162"/>
     </row>
     <row r="43" spans="1:11" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="169" t="s">
+      <c r="A43" s="163" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="169"/>
-      <c r="C43" s="169"/>
-      <c r="D43" s="169"/>
-      <c r="E43" s="169"/>
-      <c r="F43" s="169"/>
-      <c r="G43" s="169"/>
-      <c r="H43" s="169"/>
-      <c r="I43" s="169"/>
-      <c r="J43" s="169"/>
-      <c r="K43" s="169"/>
+      <c r="B43" s="163"/>
+      <c r="C43" s="163"/>
+      <c r="D43" s="163"/>
+      <c r="E43" s="163"/>
+      <c r="F43" s="163"/>
+      <c r="G43" s="163"/>
+      <c r="H43" s="163"/>
+      <c r="I43" s="163"/>
+      <c r="J43" s="163"/>
+      <c r="K43" s="163"/>
     </row>
     <row r="44" spans="1:11" s="71" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="165" t="s">
+      <c r="A44" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="165"/>
-      <c r="C44" s="165"/>
-      <c r="D44" s="165"/>
-      <c r="E44" s="165"/>
-      <c r="F44" s="165"/>
-      <c r="G44" s="165"/>
-      <c r="H44" s="165"/>
-      <c r="I44" s="165"/>
-      <c r="J44" s="165"/>
-      <c r="K44" s="165"/>
+      <c r="B44" s="159"/>
+      <c r="C44" s="159"/>
+      <c r="D44" s="159"/>
+      <c r="E44" s="159"/>
+      <c r="F44" s="159"/>
+      <c r="G44" s="159"/>
+      <c r="H44" s="159"/>
+      <c r="I44" s="159"/>
+      <c r="J44" s="159"/>
+      <c r="K44" s="159"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="161" t="s">
+      <c r="A46" s="166" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="161"/>
-      <c r="C46" s="161"/>
-      <c r="D46" s="161"/>
-      <c r="E46" s="161"/>
-      <c r="F46" s="161"/>
-      <c r="G46" s="161"/>
-      <c r="H46" s="161"/>
-      <c r="I46" s="161"/>
-      <c r="J46" s="161"/>
-      <c r="K46" s="161"/>
+      <c r="B46" s="166"/>
+      <c r="C46" s="166"/>
+      <c r="D46" s="166"/>
+      <c r="E46" s="166"/>
+      <c r="F46" s="166"/>
+      <c r="G46" s="166"/>
+      <c r="H46" s="166"/>
+      <c r="I46" s="166"/>
+      <c r="J46" s="166"/>
+      <c r="K46" s="166"/>
     </row>
     <row r="47" spans="1:11" s="80" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="78" t="s">
         <v>130</v>
       </c>
       <c r="B47" s="79"/>
-      <c r="C47" s="162" t="s">
+      <c r="C47" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="162"/>
-      <c r="E47" s="162"/>
-      <c r="F47" s="162"/>
-      <c r="G47" s="162"/>
-      <c r="H47" s="162"/>
-      <c r="I47" s="162"/>
-      <c r="J47" s="162"/>
-      <c r="K47" s="162"/>
+      <c r="D47" s="167"/>
+      <c r="E47" s="167"/>
+      <c r="F47" s="167"/>
+      <c r="G47" s="167"/>
+      <c r="H47" s="167"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="167"/>
+      <c r="K47" s="167"/>
     </row>
     <row r="48" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="163"/>
-      <c r="B48" s="159" t="s">
+      <c r="A48" s="168"/>
+      <c r="B48" s="164" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="159" t="s">
+      <c r="C48" s="164" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="159" t="s">
+      <c r="D48" s="164" t="s">
         <v>134</v>
       </c>
-      <c r="E48" s="159" t="s">
+      <c r="E48" s="164" t="s">
         <v>103</v>
       </c>
-      <c r="F48" s="159" t="s">
+      <c r="F48" s="164" t="s">
         <v>135</v>
       </c>
-      <c r="G48" s="159" t="s">
+      <c r="G48" s="164" t="s">
         <v>107</v>
       </c>
-      <c r="H48" s="164" t="s">
+      <c r="H48" s="169" t="s">
         <v>136</v>
       </c>
-      <c r="I48" s="164"/>
-      <c r="J48" s="164"/>
-      <c r="K48" s="164"/>
+      <c r="I48" s="169"/>
+      <c r="J48" s="169"/>
+      <c r="K48" s="169"/>
     </row>
     <row r="49" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="163"/>
-      <c r="B49" s="159"/>
-      <c r="C49" s="159"/>
-      <c r="D49" s="159"/>
-      <c r="E49" s="159"/>
-      <c r="F49" s="159"/>
-      <c r="G49" s="159"/>
-      <c r="H49" s="159" t="s">
+      <c r="A49" s="168"/>
+      <c r="B49" s="164"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="164"/>
+      <c r="E49" s="164"/>
+      <c r="F49" s="164"/>
+      <c r="G49" s="164"/>
+      <c r="H49" s="164" t="s">
         <v>137</v>
       </c>
-      <c r="I49" s="159"/>
+      <c r="I49" s="164"/>
       <c r="J49" s="81" t="s">
         <v>138</v>
       </c>
@@ -10521,8 +10521,8 @@
       <c r="G50" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="H50" s="160"/>
-      <c r="I50" s="160"/>
+      <c r="H50" s="165"/>
+      <c r="I50" s="165"/>
       <c r="J50" s="88"/>
       <c r="K50" s="88" t="s">
         <v>141</v>
@@ -10669,8 +10669,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="86"/>
-      <c r="H59" s="160"/>
-      <c r="I59" s="160"/>
+      <c r="H59" s="165"/>
+      <c r="I59" s="165"/>
       <c r="J59" s="88"/>
       <c r="K59" s="88"/>
     </row>
@@ -10685,19 +10685,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="86"/>
-      <c r="H60" s="160"/>
-      <c r="I60" s="160"/>
+      <c r="H60" s="165"/>
+      <c r="I60" s="165"/>
       <c r="J60" s="88"/>
       <c r="K60" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A43:K43"/>
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="H50:I50"/>
     <mergeCell ref="H59:I59"/>
@@ -10712,6 +10706,12 @@
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:K48"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
     <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Implementar um prototipo de UC1
</commit_message>
<xml_diff>
--- a/6.Gerenciamento de Projeto/SYLF - Planejamento e Controle do Projeto.xlsx
+++ b/6.Gerenciamento de Projeto/SYLF - Planejamento e Controle do Projeto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\School\6 semestre\ESO\SYLF\6.Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567BFDEA-D5D0-483A-8A76-55BBAC6CBE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5330920D-5FC9-4E88-B73A-4CA63B0FBBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{31237A52-FFD1-4E1D-B5BB-391D11929C61}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="6" xr2:uid="{31237A52-FFD1-4E1D-B5BB-391D11929C61}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -4741,7 +4741,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="231">
   <si>
     <t>Equipe</t>
   </si>
@@ -5200,11 +5200,6 @@
     <t>Atrasar a entrega do sistema</t>
   </si>
   <si>
-    <t>1. Executar horas-extras
-2. Contratar mais pessoas
-3. Renegociar prazo final</t>
-  </si>
-  <si>
     <t>APF (Método de estimativa de tamanho de sistema)</t>
   </si>
   <si>
@@ -5524,6 +5519,9 @@
   </si>
   <si>
     <t>Desenvolver o UC3 - Alterar valores de variáveis de código de modo sem fio.</t>
+  </si>
+  <si>
+    <t>Aumentar carga horária de 20 horas para 30 horas por semana.</t>
   </si>
 </sst>
 </file>
@@ -5931,7 +5929,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -6081,6 +6079,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -6104,7 +6117,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6511,10 +6524,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="40" fillId="9" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="41" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -6529,18 +6538,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="7" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -6561,24 +6558,24 @@
     <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="5" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="5" borderId="7" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="27" fillId="5" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6590,21 +6587,6 @@
     </xf>
     <xf numFmtId="164" fontId="28" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="14" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="32" fillId="15" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6620,6 +6602,21 @@
     <xf numFmtId="164" fontId="32" fillId="15" borderId="4" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="31" fillId="12" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="10" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="14" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="13" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6649,6 +6646,29 @@
     </xf>
     <xf numFmtId="164" fontId="30" fillId="6" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="9" borderId="4" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="9" borderId="4" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="3" borderId="9" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="40" fillId="9" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="24" fillId="9" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="40" fillId="9" borderId="13" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -8557,18 +8577,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
     </row>
     <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="139" t="s">
-        <v>216</v>
-      </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="139"/>
+      <c r="A2" s="138" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -8586,10 +8606,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -8597,10 +8617,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -8608,10 +8628,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -8687,7 +8707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6C5642-BF97-4AFF-B370-04CC3D024494}">
   <dimension ref="A1:AMJ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -8708,38 +8728,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="144" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="F1" s="140" t="s">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="F1" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
-      <c r="K1" s="140"/>
-      <c r="L1" s="140"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
     </row>
     <row r="2" spans="1:1024" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="141" t="s">
+      <c r="A2" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="F2" s="142" t="s">
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="F2" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
     </row>
     <row r="3" spans="1:1024" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8760,20 +8780,20 @@
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="143" t="s">
+      <c r="H3" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
+      <c r="K3" s="148"/>
+      <c r="L3" s="148"/>
     </row>
     <row r="4" spans="1:1024" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="144"/>
-      <c r="C4" s="144"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="139"/>
       <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
@@ -8816,7 +8836,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H5" s="15">
         <v>10</v>
@@ -8852,7 +8872,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H6" s="15">
         <v>10</v>
@@ -8888,7 +8908,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="127" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H7" s="128">
         <v>10</v>
@@ -8971,11 +8991,11 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="144"/>
-      <c r="C11" s="144"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
       <c r="D11" s="8">
         <f>SUM(D5:D10)</f>
         <v>25</v>
@@ -9059,7 +9079,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="131" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D15" s="13">
         <v>4</v>
@@ -9080,7 +9100,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="132" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D16" s="13">
         <v>6</v>
@@ -9101,7 +9121,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="130" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D17" s="13">
         <v>3</v>
@@ -9122,7 +9142,7 @@
         <v>31</v>
       </c>
       <c r="C18" s="130" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D18" s="13">
         <v>6</v>
@@ -9174,11 +9194,11 @@
       <c r="L20" s="19"/>
     </row>
     <row r="21" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="145" t="s">
+      <c r="A21" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="146"/>
-      <c r="C21" s="147"/>
+      <c r="B21" s="141"/>
+      <c r="C21" s="142"/>
       <c r="D21" s="8">
         <f>SUM(D12:D20)</f>
         <v>57</v>
@@ -9216,7 +9236,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D23" s="13">
         <v>8</v>
@@ -9230,7 +9250,7 @@
         <v>37</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D24" s="13">
         <v>8</v>
@@ -9244,7 +9264,7 @@
         <v>37</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D25" s="13">
         <v>8</v>
@@ -9279,11 +9299,11 @@
       </c>
     </row>
     <row r="28" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="144" t="s">
+      <c r="A28" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
+      <c r="B28" s="139"/>
+      <c r="C28" s="139"/>
       <c r="D28" s="8">
         <f>SUM(D22:D27)</f>
         <v>30</v>
@@ -9416,9 +9436,9 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="148"/>
-      <c r="B38" s="148"/>
-      <c r="C38" s="148"/>
+      <c r="A38" s="143"/>
+      <c r="B38" s="143"/>
+      <c r="C38" s="143"/>
       <c r="D38" s="8">
         <f>SUM(D29:D37)</f>
         <v>35</v>
@@ -9432,16 +9452,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="1.1437007874015752" bottom="1.1437007874015752" header="0.75000000000000011" footer="0.75000000000000011"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -9469,19 +9489,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
     </row>
     <row r="2" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="150" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
+      <c r="B3" s="150"/>
+      <c r="C3" s="150"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
@@ -9500,7 +9520,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="27">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>51</v>
@@ -9523,7 +9543,7 @@
         <v>54</v>
       </c>
       <c r="B7" s="29">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>49</v>
@@ -9535,7 +9555,7 @@
       </c>
       <c r="B8" s="30">
         <f>B6*B7*2</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>49</v>
@@ -9547,7 +9567,7 @@
       </c>
       <c r="B9" s="32">
         <f>B11/2</f>
-        <v>5.1450000000000005</v>
+        <v>3.92</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>57</v>
@@ -9559,7 +9579,7 @@
       </c>
       <c r="B10" s="32">
         <f>B4+(B4*B5)</f>
-        <v>205.8</v>
+        <v>235.2</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>49</v>
@@ -9571,7 +9591,7 @@
       </c>
       <c r="B11" s="30">
         <f>B10/B8*2</f>
-        <v>10.290000000000001</v>
+        <v>7.84</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>60</v>
@@ -9583,18 +9603,18 @@
       </c>
       <c r="B12" s="34">
         <f>B11/4</f>
-        <v>2.5725000000000002</v>
+        <v>1.96</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="151" t="s">
+      <c r="A14" s="150" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="151"/>
-      <c r="C14" s="151"/>
+      <c r="B14" s="150"/>
+      <c r="C14" s="150"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
@@ -9611,7 +9631,7 @@
       </c>
       <c r="B16" s="37">
         <f>B10*B15</f>
-        <v>4116</v>
+        <v>4704</v>
       </c>
       <c r="C16" s="36"/>
     </row>
@@ -9630,7 +9650,7 @@
       </c>
       <c r="B18" s="38">
         <f>B16*B17</f>
-        <v>823.2</v>
+        <v>940.80000000000007</v>
       </c>
       <c r="C18" s="36"/>
     </row>
@@ -9640,7 +9660,7 @@
       </c>
       <c r="B19" s="40">
         <f>B16+B18</f>
-        <v>4939.2</v>
+        <v>5644.8</v>
       </c>
       <c r="C19" s="36"/>
     </row>
@@ -9659,7 +9679,7 @@
       </c>
       <c r="B21" s="41">
         <f>B19*B20</f>
-        <v>987.84</v>
+        <v>1128.96</v>
       </c>
       <c r="C21" s="36"/>
     </row>
@@ -9669,7 +9689,7 @@
       </c>
       <c r="B22" s="40">
         <f>B19+B21</f>
-        <v>5927.04</v>
+        <v>6773.76</v>
       </c>
       <c r="C22" s="36"/>
     </row>
@@ -9691,7 +9711,7 @@
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9708,54 +9728,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="151" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="151"/>
+      <c r="K1" s="151"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="152" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
       <c r="E2" s="42">
         <f>Planejamento!$B$10</f>
-        <v>205.8</v>
+        <v>235.2</v>
       </c>
       <c r="F2" s="43"/>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="152" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
       <c r="K2" s="42"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
-      <c r="C3" s="157" t="s">
+      <c r="C3" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
       <c r="F3" s="46"/>
-      <c r="G3" s="158" t="s">
+      <c r="G3" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="158"/>
-      <c r="I3" s="158"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
       <c r="J3" s="48"/>
       <c r="K3" s="49"/>
     </row>
@@ -9802,19 +9822,19 @@
         <v>84</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" s="134">
         <v>45904</v>
       </c>
-      <c r="E5" s="135">
+      <c r="E5" s="179">
         <v>25</v>
       </c>
-      <c r="F5" s="136" t="s">
+      <c r="F5" s="135" t="s">
         <v>85</v>
       </c>
       <c r="G5" s="134" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H5" s="134">
         <v>45904</v>
@@ -9827,26 +9847,26 @@
         <v>1</v>
       </c>
       <c r="K5" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="51">
         <v>2</v>
       </c>
-      <c r="B6" s="137" t="s">
-        <v>219</v>
+      <c r="B6" s="136" t="s">
+        <v>218</v>
       </c>
       <c r="C6" s="134">
-        <v>45904</v>
-      </c>
-      <c r="D6" s="134">
-        <v>45932</v>
-      </c>
-      <c r="E6" s="152">
-        <v>125</v>
-      </c>
-      <c r="F6" s="136" t="s">
+        <v>45925</v>
+      </c>
+      <c r="D6" s="176">
+        <v>45939</v>
+      </c>
+      <c r="E6" s="181">
+        <v>60</v>
+      </c>
+      <c r="F6" s="178" t="s">
         <v>86</v>
       </c>
       <c r="G6" s="52"/>
@@ -9859,19 +9879,11 @@
       <c r="A7" s="51">
         <v>3</v>
       </c>
-      <c r="B7" s="133" t="s">
-        <v>220</v>
-      </c>
-      <c r="C7" s="134">
-        <v>45932</v>
-      </c>
-      <c r="D7" s="134">
-        <v>45946</v>
-      </c>
-      <c r="E7" s="153"/>
-      <c r="F7" s="136" t="s">
-        <v>86</v>
-      </c>
+      <c r="B7" s="133"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="178"/>
       <c r="G7" s="52"/>
       <c r="H7" s="52"/>
       <c r="I7" s="56"/>
@@ -9882,19 +9894,11 @@
       <c r="A8" s="51">
         <v>4</v>
       </c>
-      <c r="B8" s="58" t="s">
-        <v>221</v>
-      </c>
-      <c r="C8" s="59">
-        <v>45946</v>
-      </c>
-      <c r="D8" s="59">
-        <v>45960</v>
-      </c>
-      <c r="E8" s="154"/>
-      <c r="F8" s="136" t="s">
-        <v>86</v>
-      </c>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="178"/>
       <c r="G8" s="59"/>
       <c r="H8" s="59"/>
       <c r="I8" s="60"/>
@@ -9905,21 +9909,11 @@
       <c r="A9" s="51">
         <v>5</v>
       </c>
-      <c r="B9" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="59">
-        <v>45960</v>
-      </c>
-      <c r="D9" s="59">
-        <v>45974</v>
-      </c>
-      <c r="E9" s="60">
-        <v>35</v>
-      </c>
-      <c r="F9" s="136" t="s">
-        <v>86</v>
-      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="180"/>
+      <c r="F9" s="135"/>
       <c r="G9" s="59"/>
       <c r="H9" s="59"/>
       <c r="I9" s="60"/>
@@ -10008,7 +10002,7 @@
       <c r="D15" s="65"/>
       <c r="E15" s="67">
         <f>SUM(E5:E14)</f>
-        <v>185</v>
+        <v>85</v>
       </c>
       <c r="F15" s="65"/>
       <c r="G15" s="68"/>
@@ -10027,8 +10021,7 @@
       <c r="J16" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E6:E8"/>
+  <mergeCells count="5">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="G2:J2"/>
@@ -10077,15 +10070,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000B64FE-1B63-401C-B573-13BE1BFD24E2}">
   <dimension ref="A1:AMJ60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.625" style="72" customWidth="1"/>
     <col min="2" max="2" width="35.625" style="72" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="72" customWidth="1"/>
+    <col min="3" max="3" width="5.375" style="72" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.25" style="72" customWidth="1"/>
     <col min="5" max="5" width="8.875" style="72" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="72" customWidth="1"/>
@@ -10139,19 +10132,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="71" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="151"/>
+      <c r="K1" s="151"/>
     </row>
     <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -10305,10 +10298,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="160" t="s">
+      <c r="D33" s="162" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="160"/>
+      <c r="E33" s="162"/>
     </row>
     <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="D34" s="74">
@@ -10360,137 +10353,137 @@
     </row>
     <row r="40" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:11" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="161" t="s">
+      <c r="A41" s="163" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="161"/>
-      <c r="C41" s="161"/>
-      <c r="D41" s="161"/>
-      <c r="E41" s="161"/>
-      <c r="F41" s="161"/>
-      <c r="G41" s="161"/>
-      <c r="H41" s="161"/>
-      <c r="I41" s="161"/>
-      <c r="J41" s="161"/>
-      <c r="K41" s="161"/>
+      <c r="B41" s="163"/>
+      <c r="C41" s="163"/>
+      <c r="D41" s="163"/>
+      <c r="E41" s="163"/>
+      <c r="F41" s="163"/>
+      <c r="G41" s="163"/>
+      <c r="H41" s="163"/>
+      <c r="I41" s="163"/>
+      <c r="J41" s="163"/>
+      <c r="K41" s="163"/>
     </row>
     <row r="42" spans="1:11" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="162" t="s">
+      <c r="A42" s="164" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="162"/>
-      <c r="C42" s="162"/>
-      <c r="D42" s="162"/>
-      <c r="E42" s="162"/>
-      <c r="F42" s="162"/>
-      <c r="G42" s="162"/>
-      <c r="H42" s="162"/>
-      <c r="I42" s="162"/>
-      <c r="J42" s="162"/>
-      <c r="K42" s="162"/>
+      <c r="B42" s="164"/>
+      <c r="C42" s="164"/>
+      <c r="D42" s="164"/>
+      <c r="E42" s="164"/>
+      <c r="F42" s="164"/>
+      <c r="G42" s="164"/>
+      <c r="H42" s="164"/>
+      <c r="I42" s="164"/>
+      <c r="J42" s="164"/>
+      <c r="K42" s="164"/>
     </row>
     <row r="43" spans="1:11" s="71" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="163" t="s">
+      <c r="A43" s="165" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="163"/>
-      <c r="C43" s="163"/>
-      <c r="D43" s="163"/>
-      <c r="E43" s="163"/>
-      <c r="F43" s="163"/>
-      <c r="G43" s="163"/>
-      <c r="H43" s="163"/>
-      <c r="I43" s="163"/>
-      <c r="J43" s="163"/>
-      <c r="K43" s="163"/>
+      <c r="B43" s="165"/>
+      <c r="C43" s="165"/>
+      <c r="D43" s="165"/>
+      <c r="E43" s="165"/>
+      <c r="F43" s="165"/>
+      <c r="G43" s="165"/>
+      <c r="H43" s="165"/>
+      <c r="I43" s="165"/>
+      <c r="J43" s="165"/>
+      <c r="K43" s="165"/>
     </row>
     <row r="44" spans="1:11" s="71" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="159" t="s">
+      <c r="A44" s="161" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="159"/>
-      <c r="C44" s="159"/>
-      <c r="D44" s="159"/>
-      <c r="E44" s="159"/>
-      <c r="F44" s="159"/>
-      <c r="G44" s="159"/>
-      <c r="H44" s="159"/>
-      <c r="I44" s="159"/>
-      <c r="J44" s="159"/>
-      <c r="K44" s="159"/>
+      <c r="B44" s="161"/>
+      <c r="C44" s="161"/>
+      <c r="D44" s="161"/>
+      <c r="E44" s="161"/>
+      <c r="F44" s="161"/>
+      <c r="G44" s="161"/>
+      <c r="H44" s="161"/>
+      <c r="I44" s="161"/>
+      <c r="J44" s="161"/>
+      <c r="K44" s="161"/>
     </row>
     <row r="45" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="166" t="s">
+      <c r="A46" s="157" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="166"/>
-      <c r="C46" s="166"/>
-      <c r="D46" s="166"/>
-      <c r="E46" s="166"/>
-      <c r="F46" s="166"/>
-      <c r="G46" s="166"/>
-      <c r="H46" s="166"/>
-      <c r="I46" s="166"/>
-      <c r="J46" s="166"/>
-      <c r="K46" s="166"/>
+      <c r="B46" s="157"/>
+      <c r="C46" s="157"/>
+      <c r="D46" s="157"/>
+      <c r="E46" s="157"/>
+      <c r="F46" s="157"/>
+      <c r="G46" s="157"/>
+      <c r="H46" s="157"/>
+      <c r="I46" s="157"/>
+      <c r="J46" s="157"/>
+      <c r="K46" s="157"/>
     </row>
     <row r="47" spans="1:11" s="80" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="78" t="s">
         <v>130</v>
       </c>
       <c r="B47" s="79"/>
-      <c r="C47" s="167" t="s">
+      <c r="C47" s="158" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="167"/>
-      <c r="E47" s="167"/>
-      <c r="F47" s="167"/>
-      <c r="G47" s="167"/>
-      <c r="H47" s="167"/>
-      <c r="I47" s="167"/>
-      <c r="J47" s="167"/>
-      <c r="K47" s="167"/>
+      <c r="D47" s="158"/>
+      <c r="E47" s="158"/>
+      <c r="F47" s="158"/>
+      <c r="G47" s="158"/>
+      <c r="H47" s="158"/>
+      <c r="I47" s="158"/>
+      <c r="J47" s="158"/>
+      <c r="K47" s="158"/>
     </row>
     <row r="48" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="168"/>
-      <c r="B48" s="164" t="s">
+      <c r="A48" s="159"/>
+      <c r="B48" s="155" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="164" t="s">
+      <c r="C48" s="155" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="164" t="s">
+      <c r="D48" s="155" t="s">
         <v>134</v>
       </c>
-      <c r="E48" s="164" t="s">
+      <c r="E48" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="F48" s="164" t="s">
+      <c r="F48" s="155" t="s">
         <v>135</v>
       </c>
-      <c r="G48" s="164" t="s">
+      <c r="G48" s="155" t="s">
         <v>107</v>
       </c>
-      <c r="H48" s="169" t="s">
+      <c r="H48" s="160" t="s">
         <v>136</v>
       </c>
-      <c r="I48" s="169"/>
-      <c r="J48" s="169"/>
-      <c r="K48" s="169"/>
+      <c r="I48" s="160"/>
+      <c r="J48" s="160"/>
+      <c r="K48" s="160"/>
     </row>
     <row r="49" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="168"/>
-      <c r="B49" s="164"/>
-      <c r="C49" s="164"/>
-      <c r="D49" s="164"/>
-      <c r="E49" s="164"/>
-      <c r="F49" s="164"/>
-      <c r="G49" s="164"/>
-      <c r="H49" s="164" t="s">
+      <c r="A49" s="159"/>
+      <c r="B49" s="155"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="155"/>
+      <c r="E49" s="155"/>
+      <c r="F49" s="155"/>
+      <c r="G49" s="155"/>
+      <c r="H49" s="155" t="s">
         <v>137</v>
       </c>
-      <c r="I49" s="164"/>
+      <c r="I49" s="155"/>
       <c r="J49" s="81" t="s">
         <v>138</v>
       </c>
@@ -10506,7 +10499,7 @@
         <v>140</v>
       </c>
       <c r="C50" s="85">
-        <v>43891</v>
+        <v>45911</v>
       </c>
       <c r="D50" s="86" t="s">
         <v>101</v>
@@ -10519,14 +10512,14 @@
         <v>Média</v>
       </c>
       <c r="G50" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="H50" s="165"/>
-      <c r="I50" s="165"/>
-      <c r="J50" s="88"/>
-      <c r="K50" s="88" t="s">
-        <v>141</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="H50" s="156"/>
+      <c r="I50" s="156"/>
+      <c r="J50" s="88" t="s">
+        <v>230</v>
+      </c>
+      <c r="K50" s="88"/>
     </row>
     <row r="51" spans="1:11" s="82" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="83"/>
@@ -10669,8 +10662,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G59" s="86"/>
-      <c r="H59" s="165"/>
-      <c r="I59" s="165"/>
+      <c r="H59" s="156"/>
+      <c r="I59" s="156"/>
       <c r="J59" s="88"/>
       <c r="K59" s="88"/>
     </row>
@@ -10685,13 +10678,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="G60" s="86"/>
-      <c r="H60" s="165"/>
-      <c r="I60" s="165"/>
+      <c r="H60" s="156"/>
+      <c r="I60" s="156"/>
       <c r="J60" s="88"/>
       <c r="K60" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="H50:I50"/>
     <mergeCell ref="H59:I59"/>
@@ -10706,12 +10705,6 @@
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:K48"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A43:K43"/>
   </mergeCells>
   <conditionalFormatting sqref="F50:F60">
     <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
@@ -10774,167 +10767,167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="71" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="168" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+    </row>
+    <row r="2" spans="1:23" s="91" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="169" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="169"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+    </row>
+    <row r="3" spans="1:23" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="170" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="172"/>
-      <c r="K1" s="172"/>
-      <c r="L1" s="172"/>
-      <c r="M1" s="172"/>
-      <c r="N1" s="172"/>
-    </row>
-    <row r="2" spans="1:23" s="91" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="173" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="173"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="173"/>
-      <c r="M2" s="173"/>
-      <c r="N2" s="173"/>
-    </row>
-    <row r="3" spans="1:23" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="174" t="s">
+      <c r="B3" s="170"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
+      <c r="H3" s="170"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="170"/>
+    </row>
+    <row r="4" spans="1:23" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="171" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="174"/>
-      <c r="H3" s="174"/>
-      <c r="I3" s="174"/>
-      <c r="J3" s="174"/>
-      <c r="K3" s="174"/>
-      <c r="L3" s="174"/>
-      <c r="M3" s="174"/>
-      <c r="N3" s="174"/>
-    </row>
-    <row r="4" spans="1:23" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="175" t="s">
+      <c r="B4" s="171"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="171"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
+    </row>
+    <row r="5" spans="1:23" s="91" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="172" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="175"/>
-      <c r="C4" s="175"/>
-      <c r="D4" s="175"/>
-      <c r="E4" s="175"/>
-      <c r="F4" s="175"/>
-      <c r="G4" s="175"/>
-      <c r="H4" s="175"/>
-      <c r="I4" s="175"/>
-      <c r="J4" s="175"/>
-      <c r="K4" s="175"/>
-      <c r="L4" s="175"/>
-      <c r="M4" s="175"/>
-      <c r="N4" s="175"/>
-    </row>
-    <row r="5" spans="1:23" s="91" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="176" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="176"/>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="176"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="176"/>
-      <c r="H5" s="176"/>
-      <c r="I5" s="176"/>
-      <c r="J5" s="176"/>
-      <c r="K5" s="176"/>
-      <c r="L5" s="176"/>
-      <c r="M5" s="176"/>
-      <c r="N5" s="176"/>
+      <c r="B5" s="172"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="172"/>
+      <c r="I5" s="172"/>
+      <c r="J5" s="172"/>
+      <c r="K5" s="172"/>
+      <c r="L5" s="172"/>
+      <c r="M5" s="172"/>
+      <c r="N5" s="172"/>
     </row>
     <row r="6" spans="1:23" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:23" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="170" t="s">
+      <c r="A7" s="166" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="166"/>
+      <c r="D7" s="166" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="170"/>
-      <c r="D7" s="170" t="s">
+      <c r="E7" s="166"/>
+      <c r="G7" s="166" t="s">
         <v>147</v>
       </c>
-      <c r="E7" s="170"/>
-      <c r="G7" s="170" t="s">
+      <c r="H7" s="166"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
+      <c r="M7" s="166" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="170"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="170"/>
-      <c r="K7" s="170"/>
-      <c r="M7" s="170" t="s">
-        <v>149</v>
-      </c>
-      <c r="N7" s="170"/>
+      <c r="N7" s="166"/>
     </row>
     <row r="8" spans="1:23" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="94" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="95" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="D8" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="94" t="s">
+      <c r="E8" s="95" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="95" t="s">
-        <v>151</v>
-      </c>
-      <c r="G8" s="94" t="s">
+      <c r="H8" s="94" t="s">
         <v>153</v>
-      </c>
-      <c r="H8" s="94" t="s">
-        <v>154</v>
       </c>
       <c r="I8" s="94" t="s">
         <v>101</v>
       </c>
       <c r="J8" s="95" t="s">
+        <v>154</v>
+      </c>
+      <c r="K8" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="K8" s="95" t="s">
+      <c r="M8" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="M8" s="95" t="s">
+      <c r="N8" s="95" t="s">
         <v>157</v>
-      </c>
-      <c r="N8" s="95" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A9" s="92" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="92" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="93" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" s="92" t="s">
+      <c r="E9" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="94" t="s">
         <v>160</v>
-      </c>
-      <c r="E9" s="93" t="s">
-        <v>154</v>
-      </c>
-      <c r="G9" s="94" t="s">
-        <v>161</v>
       </c>
       <c r="H9" s="92">
         <v>2</v>
@@ -10950,21 +10943,21 @@
         <v>8</v>
       </c>
       <c r="M9" s="96" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N9" s="97"/>
     </row>
     <row r="10" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A10" s="92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" s="93" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" s="92"/>
       <c r="E10" s="93"/>
       <c r="G10" s="94" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H10" s="92"/>
       <c r="I10" s="92"/>
@@ -10974,7 +10967,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="96" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N10" s="97"/>
     </row>
@@ -10983,15 +10976,15 @@
       <c r="B11" s="93"/>
       <c r="D11" s="92"/>
       <c r="E11" s="93"/>
-      <c r="G11" s="170" t="s">
+      <c r="G11" s="166" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" s="166"/>
+      <c r="I11" s="166"/>
+      <c r="J11" s="166"/>
+      <c r="K11" s="166"/>
+      <c r="M11" s="96" t="s">
         <v>166</v>
-      </c>
-      <c r="H11" s="170"/>
-      <c r="I11" s="170"/>
-      <c r="J11" s="170"/>
-      <c r="K11" s="170"/>
-      <c r="M11" s="96" t="s">
-        <v>167</v>
       </c>
       <c r="N11" s="97"/>
     </row>
@@ -11001,22 +10994,22 @@
       <c r="D12" s="92"/>
       <c r="E12" s="93"/>
       <c r="G12" s="94" t="s">
+        <v>152</v>
+      </c>
+      <c r="H12" s="94" t="s">
         <v>153</v>
-      </c>
-      <c r="H12" s="94" t="s">
-        <v>154</v>
       </c>
       <c r="I12" s="94" t="s">
         <v>101</v>
       </c>
       <c r="J12" s="95" t="s">
+        <v>154</v>
+      </c>
+      <c r="K12" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="K12" s="95" t="s">
-        <v>156</v>
-      </c>
       <c r="M12" s="96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N12" s="97"/>
     </row>
@@ -11026,7 +11019,7 @@
       <c r="D13" s="92"/>
       <c r="E13" s="93"/>
       <c r="G13" s="94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H13" s="92">
         <v>1</v>
@@ -11038,11 +11031,11 @@
         <v>3</v>
       </c>
       <c r="M13" s="96" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N13" s="97"/>
       <c r="W13" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:23" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11051,7 +11044,7 @@
       <c r="D14" s="92"/>
       <c r="E14" s="93"/>
       <c r="G14" s="94" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H14" s="92"/>
       <c r="I14" s="92"/>
@@ -11061,7 +11054,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="96" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N14" s="97"/>
     </row>
@@ -11071,7 +11064,7 @@
       <c r="D15" s="92"/>
       <c r="E15" s="93"/>
       <c r="G15" s="94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H15" s="92">
         <v>1</v>
@@ -11083,7 +11076,7 @@
         <v>3</v>
       </c>
       <c r="M15" s="96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N15" s="97"/>
     </row>
@@ -11092,18 +11085,18 @@
       <c r="B16" s="93"/>
       <c r="D16" s="92"/>
       <c r="E16" s="93"/>
-      <c r="G16" s="171" t="s">
-        <v>176</v>
-      </c>
-      <c r="H16" s="171"/>
-      <c r="I16" s="171"/>
-      <c r="J16" s="171"/>
+      <c r="G16" s="167" t="s">
+        <v>175</v>
+      </c>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
       <c r="K16" s="98">
         <f>SUM(K9,K10,K13,K14,K15)</f>
         <v>14</v>
       </c>
       <c r="M16" s="96" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N16" s="97"/>
     </row>
@@ -11113,7 +11106,7 @@
       <c r="D17" s="92"/>
       <c r="E17" s="93"/>
       <c r="M17" s="96" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N17" s="97"/>
     </row>
@@ -11123,7 +11116,7 @@
       <c r="D18" s="92"/>
       <c r="E18" s="93"/>
       <c r="M18" s="96" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N18" s="97"/>
     </row>
@@ -11133,7 +11126,7 @@
       <c r="D19" s="92"/>
       <c r="E19" s="93"/>
       <c r="M19" s="96" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N19" s="97"/>
     </row>
@@ -11143,25 +11136,25 @@
       <c r="D20" s="92"/>
       <c r="E20" s="93"/>
       <c r="M20" s="96" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N20" s="97"/>
     </row>
     <row r="21" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="M21" s="96" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N21" s="97"/>
     </row>
     <row r="22" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="M22" s="96" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N22" s="97"/>
     </row>
     <row r="23" spans="1:14" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="M23" s="99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N23" s="100">
         <f>SUM(N9:N22)</f>
@@ -11170,7 +11163,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M24" s="99" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N24" s="98">
         <f>(N23*0.01)+0.65</f>
@@ -11179,7 +11172,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M25" s="99" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N25" s="101">
         <f>K16*N24</f>
@@ -11188,7 +11181,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M26" s="99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N26" s="102">
         <v>19</v>
@@ -11196,7 +11189,7 @@
     </row>
     <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="M27" s="103" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N27" s="104">
         <f>N25*N26</f>
@@ -11237,8 +11230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389CB43A-5794-4661-ACA8-D26510321904}">
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11262,73 +11255,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="172"/>
-      <c r="K1" s="172"/>
-      <c r="L1" s="172"/>
-      <c r="M1" s="172"/>
-      <c r="N1" s="172"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="178" t="s">
+      <c r="A3" s="174" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="178"/>
-      <c r="C3" s="178"/>
-      <c r="E3" s="178" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" s="178"/>
-      <c r="G3" s="178"/>
-      <c r="H3" s="178"/>
-      <c r="I3" s="178"/>
-      <c r="J3" s="178"/>
-      <c r="K3" s="178"/>
-      <c r="L3" s="178"/>
-      <c r="M3" s="178"/>
-      <c r="N3" s="178"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="E3" s="174" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="174"/>
+      <c r="J3" s="174"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="174"/>
+      <c r="M3" s="174"/>
+      <c r="N3" s="174"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="105" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="106">
-        <f>'#Estimativa-APF#'!$N$27</f>
-        <v>172.9</v>
+        <v>147</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="179" t="s">
-        <v>191</v>
-      </c>
-      <c r="F4" s="177" t="s">
+      <c r="E4" s="175" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177" t="s">
+      <c r="G4" s="173"/>
+      <c r="H4" s="173" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177" t="s">
+      <c r="I4" s="173"/>
+      <c r="J4" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177" t="s">
+      <c r="K4" s="173"/>
+      <c r="L4" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="177"/>
+      <c r="M4" s="173"/>
       <c r="N4" s="107"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -11336,68 +11328,68 @@
         <v>50</v>
       </c>
       <c r="B5" s="27">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="175"/>
+      <c r="F5" s="173" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="173"/>
+      <c r="H5" s="173" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="173"/>
+      <c r="J5" s="173" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="173"/>
+      <c r="L5" s="173" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="173"/>
+      <c r="N5" s="39" t="s">
         <v>192</v>
-      </c>
-      <c r="E5" s="179"/>
-      <c r="F5" s="177" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="177"/>
-      <c r="J5" s="177" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="177"/>
-      <c r="L5" s="177" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="177"/>
-      <c r="N5" s="39" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="108" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="109">
         <f>B4+(B4*B5)</f>
-        <v>172.9</v>
+        <v>235.2</v>
       </c>
       <c r="C6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="179"/>
+      <c r="E6" s="175"/>
       <c r="F6" s="110">
         <f>B6*G6</f>
-        <v>8.6450000000000014</v>
+        <v>11.76</v>
       </c>
       <c r="G6" s="111">
         <v>0.05</v>
       </c>
       <c r="H6" s="110">
         <f>B4*I6</f>
-        <v>34.580000000000005</v>
+        <v>29.400000000000002</v>
       </c>
       <c r="I6" s="111">
         <v>0.2</v>
       </c>
       <c r="J6" s="110">
         <f>B4*K6</f>
-        <v>112.38500000000001</v>
+        <v>95.55</v>
       </c>
       <c r="K6" s="111">
         <v>0.65</v>
       </c>
       <c r="L6" s="110">
         <f>B4*M6</f>
-        <v>17.290000000000003</v>
+        <v>14.700000000000001</v>
       </c>
       <c r="M6" s="111">
         <v>0.1</v>
@@ -11406,97 +11398,97 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" s="29">
         <v>1</v>
       </c>
       <c r="C7" s="28"/>
       <c r="E7" s="112" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F7" s="110">
         <f>F6*G7</f>
-        <v>4.7547500000000014</v>
+        <v>6.468</v>
       </c>
       <c r="G7" s="111">
         <v>0.55000000000000004</v>
       </c>
       <c r="H7" s="110">
         <f>H6*I7</f>
-        <v>10.374000000000001</v>
+        <v>8.82</v>
       </c>
       <c r="I7" s="111">
         <v>0.3</v>
       </c>
       <c r="J7" s="110">
         <f>J6*K7</f>
-        <v>13.4862</v>
+        <v>11.465999999999999</v>
       </c>
       <c r="K7" s="111">
         <v>0.12</v>
       </c>
       <c r="L7" s="110">
         <f>L6*M7</f>
-        <v>0.86450000000000016</v>
+        <v>0.7350000000000001</v>
       </c>
       <c r="M7" s="111">
         <v>0.05</v>
       </c>
       <c r="N7" s="113">
         <f>SUM(F7,H7,J7,L7)</f>
-        <v>29.47945</v>
+        <v>27.488999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="29">
+        <v>30</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="29">
-        <v>40</v>
-      </c>
-      <c r="C8" s="28" t="s">
+      <c r="E8" s="112" t="s">
         <v>198</v>
-      </c>
-      <c r="E8" s="112" t="s">
-        <v>199</v>
       </c>
       <c r="F8" s="110">
         <f>F6*G8</f>
-        <v>1.2967500000000001</v>
+        <v>1.764</v>
       </c>
       <c r="G8" s="111">
         <v>0.15</v>
       </c>
       <c r="H8" s="110">
         <f>H6*I8</f>
-        <v>6.9160000000000013</v>
+        <v>5.8800000000000008</v>
       </c>
       <c r="I8" s="111">
         <v>0.2</v>
       </c>
       <c r="J8" s="110">
         <f>J6*K8</f>
-        <v>11.238500000000002</v>
+        <v>9.5549999999999997</v>
       </c>
       <c r="K8" s="111">
         <v>0.1</v>
       </c>
       <c r="L8" s="110">
         <f>L6*M8</f>
-        <v>0.86450000000000016</v>
+        <v>0.7350000000000001</v>
       </c>
       <c r="M8" s="111">
         <v>0.05</v>
       </c>
       <c r="N8" s="113">
         <f>SUM(F8,H8,J8,L8)</f>
-        <v>20.315750000000001</v>
+        <v>17.934000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B9" s="29">
         <v>2</v>
@@ -11505,101 +11497,101 @@
         <v>60</v>
       </c>
       <c r="E9" s="112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F9" s="110">
         <f>F6*G9</f>
-        <v>0.17290000000000003</v>
+        <v>0.23519999999999999</v>
       </c>
       <c r="G9" s="111">
         <v>0.02</v>
       </c>
       <c r="H9" s="110">
         <f>H6*I9</f>
-        <v>6.9160000000000013</v>
+        <v>5.8800000000000008</v>
       </c>
       <c r="I9" s="111">
         <v>0.2</v>
       </c>
       <c r="J9" s="110">
         <f>J6*K9</f>
-        <v>44.954000000000008</v>
+        <v>38.22</v>
       </c>
       <c r="K9" s="111">
         <v>0.4</v>
       </c>
       <c r="L9" s="110">
         <f>L6*M9</f>
-        <v>2.5935000000000001</v>
+        <v>2.2050000000000001</v>
       </c>
       <c r="M9" s="111">
         <v>0.15</v>
       </c>
       <c r="N9" s="113">
         <f>SUM(F9,H9,J9,L9)</f>
-        <v>54.636400000000009</v>
+        <v>46.540199999999999</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="114" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="115">
         <f>(B7*B8)*B9</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C10" s="114" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="112" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F10" s="110">
         <f>F6*G10</f>
-        <v>0.43225000000000008</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="G10" s="111">
         <v>0.05</v>
       </c>
       <c r="H10" s="110">
         <f>H6*I10</f>
-        <v>2.7664000000000004</v>
+        <v>2.3520000000000003</v>
       </c>
       <c r="I10" s="111">
         <v>0.08</v>
       </c>
       <c r="J10" s="110">
         <f>J6*K10</f>
-        <v>11.238500000000002</v>
+        <v>9.5549999999999997</v>
       </c>
       <c r="K10" s="111">
         <v>0.1</v>
       </c>
       <c r="L10" s="110">
         <f>L6*M10</f>
-        <v>1.7290000000000003</v>
+        <v>1.4700000000000002</v>
       </c>
       <c r="M10" s="111">
         <v>0.1</v>
       </c>
       <c r="N10" s="113">
         <f>SUM(F10,H10,J10,L10)</f>
-        <v>16.166150000000002</v>
+        <v>13.965000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="105" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="116">
         <f>B6/B10*2</f>
-        <v>4.3224999999999998</v>
+        <v>7.84</v>
       </c>
       <c r="C11" s="105" t="s">
         <v>60</v>
       </c>
       <c r="E11" s="112" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F11" s="110">
         <f>F6*G11</f>
@@ -11610,47 +11602,47 @@
       </c>
       <c r="H11" s="110">
         <f>H6*I11</f>
-        <v>0.6916000000000001</v>
+        <v>0.58800000000000008</v>
       </c>
       <c r="I11" s="111">
         <v>0.02</v>
       </c>
       <c r="J11" s="110">
         <f>J6*K11</f>
-        <v>5.619250000000001</v>
+        <v>4.7774999999999999</v>
       </c>
       <c r="K11" s="111">
         <v>0.05</v>
       </c>
       <c r="L11" s="110">
         <f>L6*M11</f>
-        <v>1.7290000000000003</v>
+        <v>1.4700000000000002</v>
       </c>
       <c r="M11" s="111">
         <v>0.1</v>
       </c>
       <c r="N11" s="113">
         <f>SUM(F11,H11,J11,L11)</f>
-        <v>8.0398500000000013</v>
+        <v>6.8354999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="105" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="116">
         <f>B11/4</f>
-        <v>1.0806249999999999</v>
+        <v>1.96</v>
       </c>
       <c r="C12" s="105" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="117" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F12" s="118">
         <f t="shared" ref="F12:M12" si="0">SUM(F7:F11)</f>
-        <v>6.6566500000000017</v>
+        <v>9.0551999999999992</v>
       </c>
       <c r="G12" s="119">
         <f t="shared" si="0"/>
@@ -11658,7 +11650,7 @@
       </c>
       <c r="H12" s="118">
         <f t="shared" si="0"/>
-        <v>27.664000000000005</v>
+        <v>23.520000000000003</v>
       </c>
       <c r="I12" s="119">
         <f t="shared" si="0"/>
@@ -11666,7 +11658,7 @@
       </c>
       <c r="J12" s="118">
         <f t="shared" si="0"/>
-        <v>86.536450000000002</v>
+        <v>73.573499999999996</v>
       </c>
       <c r="K12" s="119">
         <f t="shared" si="0"/>
@@ -11674,7 +11666,7 @@
       </c>
       <c r="L12" s="118">
         <f t="shared" si="0"/>
-        <v>7.7805000000000009</v>
+        <v>6.6150000000000002</v>
       </c>
       <c r="M12" s="119">
         <f t="shared" si="0"/>
@@ -11684,95 +11676,95 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="114" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B13" s="120">
         <f>B11/B9</f>
-        <v>2.1612499999999999</v>
+        <v>3.92</v>
       </c>
       <c r="C13" s="114" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="112" t="s">
         <v>209</v>
-      </c>
-      <c r="E13" s="112" t="s">
-        <v>210</v>
       </c>
       <c r="F13" s="110">
         <f>F6*G13</f>
-        <v>0.25935000000000002</v>
+        <v>0.3528</v>
       </c>
       <c r="G13" s="111">
         <v>0.03</v>
       </c>
       <c r="H13" s="110">
         <f>H6*I13</f>
-        <v>2.7664000000000004</v>
+        <v>2.3520000000000003</v>
       </c>
       <c r="I13" s="111">
         <v>0.08</v>
       </c>
       <c r="J13" s="110">
         <f>J6*K13</f>
-        <v>14.610050000000001</v>
+        <v>12.4215</v>
       </c>
       <c r="K13" s="111">
         <v>0.13</v>
       </c>
       <c r="L13" s="110">
         <f>L6*M13</f>
-        <v>5.1870000000000003</v>
+        <v>4.41</v>
       </c>
       <c r="M13" s="111">
         <v>0.3</v>
       </c>
       <c r="N13" s="113">
         <f>SUM(F13,H13,J13,L13)</f>
-        <v>22.822800000000004</v>
+        <v>19.536300000000001</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E14" s="112" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F14" s="110">
         <f>F6*G14</f>
-        <v>1.7290000000000003</v>
+        <v>2.3519999999999999</v>
       </c>
       <c r="G14" s="111">
         <v>0.2</v>
       </c>
       <c r="H14" s="110">
         <f>H6*I14</f>
-        <v>4.1496000000000004</v>
+        <v>3.528</v>
       </c>
       <c r="I14" s="111">
         <v>0.12</v>
       </c>
       <c r="J14" s="110">
         <f>J6*K14</f>
-        <v>11.238500000000002</v>
+        <v>9.5549999999999997</v>
       </c>
       <c r="K14" s="111">
         <v>0.1</v>
       </c>
       <c r="L14" s="110">
         <f>L6*M14</f>
-        <v>4.3225000000000007</v>
+        <v>3.6750000000000003</v>
       </c>
       <c r="M14" s="111">
         <v>0.25</v>
       </c>
       <c r="N14" s="113">
         <f>SUM(F14,H14,J14,L14)</f>
-        <v>21.439600000000002</v>
+        <v>19.11</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E15" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F15" s="118">
         <f t="shared" ref="F15:M15" si="1">SUM(F13:F14)</f>
-        <v>1.9883500000000003</v>
+        <v>2.7047999999999996</v>
       </c>
       <c r="G15" s="119">
         <f t="shared" si="1"/>
@@ -11780,7 +11772,7 @@
       </c>
       <c r="H15" s="118">
         <f t="shared" si="1"/>
-        <v>6.9160000000000004</v>
+        <v>5.8800000000000008</v>
       </c>
       <c r="I15" s="119">
         <f t="shared" si="1"/>
@@ -11788,7 +11780,7 @@
       </c>
       <c r="J15" s="118">
         <f t="shared" si="1"/>
-        <v>25.848550000000003</v>
+        <v>21.976500000000001</v>
       </c>
       <c r="K15" s="119">
         <f t="shared" si="1"/>
@@ -11796,7 +11788,7 @@
       </c>
       <c r="L15" s="118">
         <f t="shared" si="1"/>
-        <v>9.509500000000001</v>
+        <v>8.0850000000000009</v>
       </c>
       <c r="M15" s="119">
         <f t="shared" si="1"/>
@@ -11805,17 +11797,17 @@
       <c r="N15" s="117"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="178" t="s">
+      <c r="A16" s="174" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="178"/>
-      <c r="C16" s="178"/>
+      <c r="B16" s="174"/>
+      <c r="C16" s="174"/>
       <c r="E16" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F16" s="121">
         <f t="shared" ref="F16:M16" si="2">F12+F15</f>
-        <v>8.6450000000000014</v>
+        <v>11.759999999999998</v>
       </c>
       <c r="G16" s="122">
         <f t="shared" si="2"/>
@@ -11823,7 +11815,7 @@
       </c>
       <c r="H16" s="121">
         <f t="shared" si="2"/>
-        <v>34.580000000000005</v>
+        <v>29.400000000000006</v>
       </c>
       <c r="I16" s="122">
         <f t="shared" si="2"/>
@@ -11831,7 +11823,7 @@
       </c>
       <c r="J16" s="121">
         <f t="shared" si="2"/>
-        <v>112.38500000000001</v>
+        <v>95.55</v>
       </c>
       <c r="K16" s="122">
         <f t="shared" si="2"/>
@@ -11839,7 +11831,7 @@
       </c>
       <c r="L16" s="121">
         <f t="shared" si="2"/>
-        <v>17.290000000000003</v>
+        <v>14.700000000000001</v>
       </c>
       <c r="M16" s="122">
         <f t="shared" si="2"/>
@@ -11847,7 +11839,7 @@
       </c>
       <c r="N16" s="123">
         <f>SUM(N7:N11,N13,N14)</f>
-        <v>172.90000000000003</v>
+        <v>151.41000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -11866,7 +11858,7 @@
       </c>
       <c r="B18" s="37">
         <f>B6*B17</f>
-        <v>3458</v>
+        <v>4704</v>
       </c>
       <c r="C18" s="36"/>
       <c r="L18" s="68"/>
@@ -11896,11 +11888,11 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21" s="125">
         <f>B18+B20</f>
-        <v>3458</v>
+        <v>4704</v>
       </c>
       <c r="C21" s="36"/>
       <c r="N21" s="68"/>
@@ -11921,17 +11913,17 @@
       </c>
       <c r="B23" s="41">
         <f>B21*B22</f>
-        <v>691.6</v>
+        <v>940.80000000000007</v>
       </c>
       <c r="C23" s="36"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="125">
         <f>B21+B23</f>
-        <v>4149.6000000000004</v>
+        <v>5644.8</v>
       </c>
       <c r="C24" s="36"/>
     </row>

</xml_diff>